<commit_message>
0225｜EASY｜Implement Stack using Queues
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1BD2F0-43E8-4143-975D-F9A3A613BEF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF665D7-F1D3-4978-A1FE-A25F3B5EF09B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="1905" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
+    <workbookView xWindow="6540" yWindow="2160" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="212">
   <si>
     <t>Date</t>
   </si>
@@ -695,6 +695,18 @@
   </si>
   <si>
     <t>sort() 方法</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Implement Stack using Queues</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0225</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>too easy..</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -784,7 +796,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -812,7 +824,6 @@
     <xf numFmtId="177" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="177" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="177" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1127,10 +1138,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914384AD-4934-744A-8C44-1EF839F36E18}">
-  <dimension ref="A1:P68"/>
+  <dimension ref="A1:P69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G59" zoomScale="150" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J71" sqref="J71"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="150" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69:XFD69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -4382,7 +4393,7 @@
       </c>
     </row>
     <row r="67" spans="1:16">
-      <c r="A67" s="19" t="s">
+      <c r="A67" s="4" t="s">
         <v>203</v>
       </c>
       <c r="B67" s="4" t="s">
@@ -4394,37 +4405,37 @@
       <c r="D67" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E67" s="10" t="s">
+      <c r="E67" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="F67" s="10" t="s">
+      <c r="F67" s="4" t="s">
         <v>207</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H67" s="18">
+      <c r="H67" s="16">
         <v>56</v>
       </c>
-      <c r="I67" s="14">
+      <c r="I67" s="12">
         <v>19.059999999999999</v>
       </c>
-      <c r="J67" s="18">
+      <c r="J67" s="16">
         <v>60</v>
       </c>
-      <c r="K67" s="14">
+      <c r="K67" s="12">
         <v>9.64</v>
       </c>
-      <c r="L67" s="24">
+      <c r="L67" s="22">
         <v>16.600000000000001</v>
       </c>
-      <c r="M67" s="14">
+      <c r="M67" s="12">
         <v>54.95</v>
       </c>
       <c r="N67" s="6">
         <v>43847</v>
       </c>
-      <c r="O67" s="25">
+      <c r="O67" s="7">
         <v>0.12986111111111112</v>
       </c>
       <c r="P67" s="20" t="b">
@@ -4432,7 +4443,7 @@
       </c>
     </row>
     <row r="68" spans="1:16">
-      <c r="A68" s="19" t="s">
+      <c r="A68" s="4" t="s">
         <v>203</v>
       </c>
       <c r="B68" s="4" t="s">
@@ -4444,42 +4455,90 @@
       <c r="D68" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E68" s="10" t="s">
+      <c r="E68" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="F68" s="10" t="s">
+      <c r="F68" s="4" t="s">
         <v>208</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H68" s="18">
+      <c r="H68" s="16">
         <v>32</v>
       </c>
-      <c r="I68" s="14">
+      <c r="I68" s="12">
         <v>88.87</v>
       </c>
-      <c r="J68" s="18">
+      <c r="J68" s="16">
         <v>32</v>
       </c>
-      <c r="K68" s="14">
+      <c r="K68" s="12">
         <v>88.87</v>
       </c>
-      <c r="L68" s="24">
+      <c r="L68" s="22">
         <v>11.3</v>
       </c>
-      <c r="M68" s="14">
+      <c r="M68" s="12">
         <v>96.7</v>
       </c>
       <c r="N68" s="6">
         <v>43847</v>
       </c>
-      <c r="O68" s="25">
+      <c r="O68" s="7">
         <v>0.12986111111111112</v>
       </c>
       <c r="P68" s="20" t="b">
         <v>0</v>
       </c>
+    </row>
+    <row r="69" spans="1:16">
+      <c r="A69" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H69" s="16">
+        <v>0</v>
+      </c>
+      <c r="I69" s="12">
+        <v>100</v>
+      </c>
+      <c r="J69" s="16">
+        <v>0</v>
+      </c>
+      <c r="K69" s="12">
+        <v>100</v>
+      </c>
+      <c r="L69" s="22">
+        <v>9.1</v>
+      </c>
+      <c r="M69" s="12">
+        <v>6.67</v>
+      </c>
+      <c r="N69" s="6">
+        <v>43847</v>
+      </c>
+      <c r="O69" s="7">
+        <v>0.14097222222222222</v>
+      </c>
+      <c r="P69" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:P47" xr:uid="{33932A4B-0B4D-2843-BDF5-66CE306FFE65}"/>

</xml_diff>

<commit_message>
0191｜EASY｜Number of 1 Bits
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8AA297-6050-4F47-90E4-08C3EFD2E76F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C7AA75-7393-45BE-84B9-5BC6DAE4EDA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6540" yWindow="2160" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$P$47</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="231">
   <si>
     <t>Date</t>
   </si>
@@ -758,7 +759,32 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>8.2 </t>
+    <t>Number of 1 Bits</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0191</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>method3.cpp</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bit Manipulation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bitset</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>换算2进制</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bitwise operator</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1189,10 +1215,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914384AD-4934-744A-8C44-1EF839F36E18}">
-  <dimension ref="A1:P73"/>
+  <dimension ref="A1:P76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="150" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="150" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -4777,8 +4803,8 @@
       <c r="K73" s="12">
         <v>6.16</v>
       </c>
-      <c r="L73" s="22" t="s">
-        <v>224</v>
+      <c r="L73" s="22">
+        <v>8.1999999999999993</v>
       </c>
       <c r="M73" s="12">
         <v>95.83</v>
@@ -4791,6 +4817,156 @@
       </c>
       <c r="P73" s="20" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16">
+      <c r="A74" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H74" s="16">
+        <v>0</v>
+      </c>
+      <c r="I74" s="12">
+        <v>100</v>
+      </c>
+      <c r="J74" s="16">
+        <v>4</v>
+      </c>
+      <c r="K74" s="12">
+        <v>66.239999999999995</v>
+      </c>
+      <c r="L74" s="22">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="M74" s="12">
+        <v>60.98</v>
+      </c>
+      <c r="N74" s="6">
+        <v>43847</v>
+      </c>
+      <c r="O74" s="7">
+        <v>0.64930555555555558</v>
+      </c>
+      <c r="P74" s="20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16">
+      <c r="A75" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H75" s="16">
+        <v>0</v>
+      </c>
+      <c r="I75" s="12">
+        <v>100</v>
+      </c>
+      <c r="J75" s="16">
+        <v>4</v>
+      </c>
+      <c r="K75" s="12">
+        <v>66.239999999999995</v>
+      </c>
+      <c r="L75" s="22">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="M75" s="12">
+        <v>78.05</v>
+      </c>
+      <c r="N75" s="6">
+        <v>43847</v>
+      </c>
+      <c r="O75" s="7">
+        <v>0.64930555555555558</v>
+      </c>
+      <c r="P75" s="20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16">
+      <c r="A76" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H76" s="16">
+        <v>0</v>
+      </c>
+      <c r="I76" s="12">
+        <v>100</v>
+      </c>
+      <c r="J76" s="16">
+        <v>4</v>
+      </c>
+      <c r="K76" s="12">
+        <v>66.239999999999995</v>
+      </c>
+      <c r="L76" s="22">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="M76" s="12">
+        <v>60.98</v>
+      </c>
+      <c r="N76" s="6">
+        <v>43847</v>
+      </c>
+      <c r="O76" s="7">
+        <v>0.64930555555555558</v>
+      </c>
+      <c r="P76" s="20" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
0083｜EASY｜Remove Duplicates from Sorted List
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C7AA75-7393-45BE-84B9-5BC6DAE4EDA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B9B0D6-3E30-4C27-BFBC-EA79A3109238}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6540" yWindow="2160" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$P$47</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="235">
   <si>
     <t>Date</t>
   </si>
@@ -784,6 +783,22 @@
   </si>
   <si>
     <t>bitwise operator</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remove Duplicates from Sorted List</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0083</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>set count</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>check 现在和下个点</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1215,10 +1230,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914384AD-4934-744A-8C44-1EF839F36E18}">
-  <dimension ref="A1:P76"/>
+  <dimension ref="A1:P78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="150" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="150" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -4969,6 +4984,106 @@
         <v>0</v>
       </c>
     </row>
+    <row r="77" spans="1:16">
+      <c r="A77" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H77" s="16">
+        <v>12</v>
+      </c>
+      <c r="I77" s="12">
+        <v>75.47</v>
+      </c>
+      <c r="J77" s="16">
+        <v>12</v>
+      </c>
+      <c r="K77" s="12">
+        <v>75.47</v>
+      </c>
+      <c r="L77" s="22">
+        <v>9.9</v>
+      </c>
+      <c r="M77" s="12">
+        <v>15.09</v>
+      </c>
+      <c r="N77" s="6">
+        <v>43847</v>
+      </c>
+      <c r="O77" s="7">
+        <v>0.86597222222222225</v>
+      </c>
+      <c r="P77" s="20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16">
+      <c r="A78" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H78" s="16">
+        <v>16</v>
+      </c>
+      <c r="I78" s="12">
+        <v>18.89</v>
+      </c>
+      <c r="J78" s="16">
+        <v>16</v>
+      </c>
+      <c r="K78" s="12">
+        <v>18.89</v>
+      </c>
+      <c r="L78" s="22">
+        <v>10.6</v>
+      </c>
+      <c r="M78" s="12">
+        <v>5.66</v>
+      </c>
+      <c r="N78" s="6">
+        <v>43847</v>
+      </c>
+      <c r="O78" s="7">
+        <v>0.86597222222222225</v>
+      </c>
+      <c r="P78" s="20" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:P47" xr:uid="{33932A4B-0B4D-2843-BDF5-66CE306FFE65}"/>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
0235｜EASY｜Lowest Common Ancestor of a Binary Search Tree
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F390E9-997B-4162-ADDD-4E3A698D4F80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DAF12FC-D884-47C2-9570-88931835548A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="3420" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
+    <workbookView xWindow="5820" yWindow="7740" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="249">
   <si>
     <t>Date</t>
   </si>
@@ -839,6 +839,22 @@
   </si>
   <si>
     <t>斐波那契数列，见pdf</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lowest Common Ancestor of a Binary Search Tree</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0235</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>随意树的路径</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>注意二叉树，左小右大，（此题每个node的值为unique）</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1270,10 +1286,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914384AD-4934-744A-8C44-1EF839F36E18}">
-  <dimension ref="A1:Q81"/>
+  <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -5290,6 +5306,111 @@
         <v>0</v>
       </c>
     </row>
+    <row r="82" spans="1:17">
+      <c r="B82" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="G82" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="H82" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I82" s="16">
+        <v>244</v>
+      </c>
+      <c r="J82" s="12">
+        <v>7.14</v>
+      </c>
+      <c r="K82" s="16">
+        <v>244</v>
+      </c>
+      <c r="L82" s="12">
+        <v>7.14</v>
+      </c>
+      <c r="M82" s="22">
+        <v>181.6</v>
+      </c>
+      <c r="N82" s="12">
+        <v>5.88</v>
+      </c>
+      <c r="O82" s="6">
+        <v>43848</v>
+      </c>
+      <c r="P82" s="7">
+        <v>3.1944444444444449E-2</v>
+      </c>
+      <c r="Q82" s="20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17">
+      <c r="B83" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="G83" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="H83" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I83" s="16">
+        <v>40</v>
+      </c>
+      <c r="J83" s="12">
+        <v>53.22</v>
+      </c>
+      <c r="K83" s="16">
+        <v>40</v>
+      </c>
+      <c r="L83" s="12">
+        <v>53.22</v>
+      </c>
+      <c r="M83" s="22">
+        <v>25.8</v>
+      </c>
+      <c r="N83" s="12">
+        <v>100</v>
+      </c>
+      <c r="O83" s="6">
+        <v>43848</v>
+      </c>
+      <c r="P83" s="7">
+        <v>3.1944444444444449E-2</v>
+      </c>
+      <c r="Q83" s="20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1048576" spans="3:3">
+      <c r="C1048576" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="B1:Q47" xr:uid="{33932A4B-0B4D-2843-BDF5-66CE306FFE65}"/>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
0111｜EASY｜Minimum Depth of Binary Tree
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DAF12FC-D884-47C2-9570-88931835548A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D89CB2-9617-48F5-B088-ADC122B85784}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="7740" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
+    <workbookView xWindow="6885" yWindow="8415" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="253">
   <si>
     <t>Date</t>
   </si>
@@ -855,6 +855,22 @@
   </si>
   <si>
     <t>注意二叉树，左小右大，（此题每个node的值为unique）</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0111</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Minimum Depth of Binary Tree</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tree｜Depth-first Search｜Breadth-first Search</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>iterate，注意一支有的时候的特殊情况</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1288,8 +1304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914384AD-4934-744A-8C44-1EF839F36E18}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView tabSelected="1" topLeftCell="G75" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H80" sqref="H80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -5406,6 +5422,56 @@
         <v>0</v>
       </c>
     </row>
+    <row r="84" spans="1:17">
+      <c r="B84" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F84" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="G84" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="H84" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I84" s="16">
+        <v>8</v>
+      </c>
+      <c r="J84" s="12">
+        <v>95.66</v>
+      </c>
+      <c r="K84" s="16">
+        <v>12</v>
+      </c>
+      <c r="L84" s="12">
+        <v>75.510000000000005</v>
+      </c>
+      <c r="M84" s="22">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="N84" s="12">
+        <v>64.28</v>
+      </c>
+      <c r="O84" s="6">
+        <v>43848</v>
+      </c>
+      <c r="P84" s="7">
+        <v>5.2777777777777778E-2</v>
+      </c>
+      <c r="Q84" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="1048576" spans="3:3">
       <c r="C1048576" s="4" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
0160｜EASY｜Intersection of Two Linked Lists
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D89CB2-9617-48F5-B088-ADC122B85784}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E9891D-B432-400C-B27E-A877B4815D6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6885" yWindow="8415" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
+    <workbookView xWindow="6270" yWindow="3810" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="257">
   <si>
     <t>Date</t>
   </si>
@@ -871,6 +871,22 @@
   </si>
   <si>
     <t>iterate，注意一支有的时候的特殊情况</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intersection of Two Linked Lists</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0160</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>set check</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>use stack</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1304,8 +1320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914384AD-4934-744A-8C44-1EF839F36E18}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G75" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H80" sqref="H80"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -5472,6 +5488,106 @@
         <v>28</v>
       </c>
     </row>
+    <row r="85" spans="1:17">
+      <c r="B85" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="G85" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="H85" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I85" s="16">
+        <v>60</v>
+      </c>
+      <c r="J85" s="12">
+        <v>24.91</v>
+      </c>
+      <c r="K85" s="16">
+        <v>68</v>
+      </c>
+      <c r="L85" s="12">
+        <v>15.16</v>
+      </c>
+      <c r="M85" s="22">
+        <v>20</v>
+      </c>
+      <c r="N85" s="12">
+        <v>12.96</v>
+      </c>
+      <c r="O85" s="6">
+        <v>43848</v>
+      </c>
+      <c r="P85" s="7">
+        <v>0.11180555555555556</v>
+      </c>
+      <c r="Q85" s="20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17">
+      <c r="B86" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="H86" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I86" s="16">
+        <v>48</v>
+      </c>
+      <c r="J86" s="12">
+        <v>83.7</v>
+      </c>
+      <c r="K86" s="16">
+        <v>52</v>
+      </c>
+      <c r="L86" s="12">
+        <v>59.97</v>
+      </c>
+      <c r="M86" s="22">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="N86" s="12">
+        <v>20.37</v>
+      </c>
+      <c r="O86" s="6">
+        <v>43848</v>
+      </c>
+      <c r="P86" s="7">
+        <v>0.11180555555555556</v>
+      </c>
+      <c r="Q86" s="20" t="b">
+        <v>0</v>
+      </c>
+    </row>
     <row r="1048576" spans="3:3">
       <c r="C1048576" s="4" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
0657｜EASY｜Robot Return to Origin
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E9891D-B432-400C-B27E-A877B4815D6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4972D1-C5D8-4A73-A183-BA161EE974AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6270" yWindow="3810" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="262">
   <si>
     <t>Date</t>
   </si>
@@ -887,6 +887,26 @@
   </si>
   <si>
     <t>use stack</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Robot Return to Origin</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0657</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>use switch</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>use +-char</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -5588,6 +5608,106 @@
         <v>0</v>
       </c>
     </row>
+    <row r="87" spans="1:17">
+      <c r="B87" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="G87" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="H87" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I87" s="16">
+        <v>16</v>
+      </c>
+      <c r="J87" s="12">
+        <v>87.7</v>
+      </c>
+      <c r="K87" s="16">
+        <v>20</v>
+      </c>
+      <c r="L87" s="12">
+        <v>39.14</v>
+      </c>
+      <c r="M87" s="22">
+        <v>10.3</v>
+      </c>
+      <c r="N87" s="12">
+        <v>36.590000000000003</v>
+      </c>
+      <c r="O87" s="6">
+        <v>43848</v>
+      </c>
+      <c r="P87" s="7">
+        <v>0.14027777777777778</v>
+      </c>
+      <c r="Q87" s="20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17">
+      <c r="B88" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="H88" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I88" s="16">
+        <v>12</v>
+      </c>
+      <c r="J88" s="12">
+        <v>96.47</v>
+      </c>
+      <c r="K88" s="16">
+        <v>16</v>
+      </c>
+      <c r="L88" s="12">
+        <v>87.7</v>
+      </c>
+      <c r="M88" s="22">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="N88" s="12">
+        <v>56.1</v>
+      </c>
+      <c r="O88" s="6">
+        <v>43848</v>
+      </c>
+      <c r="P88" s="7">
+        <v>0.14027777777777778</v>
+      </c>
+      <c r="Q88" s="20" t="b">
+        <v>0</v>
+      </c>
+    </row>
     <row r="1048576" spans="3:3">
       <c r="C1048576" s="4" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
1313｜EASY｜Decompress Run-Length Encoded List
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4972D1-C5D8-4A73-A183-BA161EE974AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B6A7EC-AF2C-4F1F-AFF4-46C43A472EFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6270" yWindow="3810" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="264">
   <si>
     <t>Date</t>
   </si>
@@ -907,6 +907,14 @@
   </si>
   <si>
     <t>use +-char</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Decompress Run-Length Encoded List</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1313</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1340,8 +1348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914384AD-4934-744A-8C44-1EF839F36E18}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89:XFD89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -5708,6 +5716,56 @@
         <v>0</v>
       </c>
     </row>
+    <row r="89" spans="1:17">
+      <c r="B89" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I89" s="16">
+        <v>44</v>
+      </c>
+      <c r="J89" s="12">
+        <v>89.16</v>
+      </c>
+      <c r="K89" s="16">
+        <v>44</v>
+      </c>
+      <c r="L89" s="12">
+        <v>89.16</v>
+      </c>
+      <c r="M89" s="22">
+        <v>10.6</v>
+      </c>
+      <c r="N89" s="12">
+        <v>100</v>
+      </c>
+      <c r="O89" s="6">
+        <v>43848</v>
+      </c>
+      <c r="P89" s="7">
+        <v>0.15902777777777777</v>
+      </c>
+      <c r="Q89" s="20" t="b">
+        <v>0</v>
+      </c>
+    </row>
     <row r="1048576" spans="3:3">
       <c r="C1048576" s="4" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
1309｜EASY｜Decrypt String from Alphabet to Integer Mapping
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B6A7EC-AF2C-4F1F-AFF4-46C43A472EFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1AF509-6ED9-4CD4-ADC7-A03ABB167AEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6270" yWindow="3810" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="268">
   <si>
     <t>Date</t>
   </si>
@@ -915,6 +915,22 @@
   </si>
   <si>
     <t>1313</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Decrypt String from Alphabet to Integer Mapping</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1309</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(char) int -&gt; char</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1349,7 +1365,7 @@
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A72" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89:XFD89"/>
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -5766,6 +5782,56 @@
         <v>0</v>
       </c>
     </row>
+    <row r="90" spans="1:17">
+      <c r="B90" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="G90" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I90" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="J90" s="12">
+        <v>100</v>
+      </c>
+      <c r="K90" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="L90" s="12">
+        <v>100</v>
+      </c>
+      <c r="M90" s="22">
+        <v>8.5</v>
+      </c>
+      <c r="N90" s="12">
+        <v>100</v>
+      </c>
+      <c r="O90" s="6">
+        <v>43848</v>
+      </c>
+      <c r="P90" s="7">
+        <v>0.18611111111111112</v>
+      </c>
+      <c r="Q90" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="1048576" spans="3:3">
       <c r="C1048576" s="4" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
1295｜EASY｜Find Numbers with Even Number of Digits
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1AF509-6ED9-4CD4-ADC7-A03ABB167AEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C17031-2A41-43EA-9E4E-48735FB7CC30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6270" yWindow="3810" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="269">
   <si>
     <t>Date</t>
   </si>
@@ -910,10 +910,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Decompress Run-Length Encoded List</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>1313</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -931,6 +927,14 @@
   </si>
   <si>
     <t>0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Find Numbers with Even Number of Digits</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1295</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1364,8 +1368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914384AD-4934-744A-8C44-1EF839F36E18}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -5734,13 +5738,13 @@
     </row>
     <row r="89" spans="1:17">
       <c r="B89" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>94</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>64</v>
@@ -5784,13 +5788,13 @@
     </row>
     <row r="90" spans="1:17">
       <c r="B90" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>94</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E90" s="4" t="s">
         <v>64</v>
@@ -5799,19 +5803,19 @@
         <v>259</v>
       </c>
       <c r="G90" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H90" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I90" s="16" t="s">
-        <v>267</v>
+      <c r="I90" s="16">
+        <v>0</v>
       </c>
       <c r="J90" s="12">
         <v>100</v>
       </c>
       <c r="K90" s="16" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="L90" s="12">
         <v>100</v>
@@ -5829,6 +5833,56 @@
         <v>0.18611111111111112</v>
       </c>
       <c r="Q90" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17">
+      <c r="B91" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G91" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I91" s="16">
+        <v>8</v>
+      </c>
+      <c r="J91" s="12">
+        <v>73.17</v>
+      </c>
+      <c r="K91" s="16">
+        <v>8</v>
+      </c>
+      <c r="L91" s="12">
+        <v>73.17</v>
+      </c>
+      <c r="M91" s="22">
+        <v>9</v>
+      </c>
+      <c r="N91" s="12">
+        <v>100</v>
+      </c>
+      <c r="O91" s="6">
+        <v>43848</v>
+      </c>
+      <c r="P91" s="7">
+        <v>0.21111111111111111</v>
+      </c>
+      <c r="Q91" s="20" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1221｜EASY｜Split a String in Balanced Strings
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C17031-2A41-43EA-9E4E-48735FB7CC30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF7852B-3775-4914-864D-6C49C2252D25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6270" yWindow="3810" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
+    <workbookView xWindow="9930" yWindow="4890" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="272">
   <si>
     <t>Date</t>
   </si>
@@ -935,6 +935,18 @@
   </si>
   <si>
     <t>1295</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Split a String in Balanced Strings</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1221</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>String｜Greedy</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1369,7 +1381,7 @@
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A75" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89"/>
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -5886,6 +5898,56 @@
         <v>32</v>
       </c>
     </row>
+    <row r="92" spans="1:17">
+      <c r="B92" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="G92" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="H92" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I92" s="16">
+        <v>4</v>
+      </c>
+      <c r="J92" s="12">
+        <v>58.71</v>
+      </c>
+      <c r="K92" s="16">
+        <v>4</v>
+      </c>
+      <c r="L92" s="12">
+        <v>58.71</v>
+      </c>
+      <c r="M92" s="22">
+        <v>8.6</v>
+      </c>
+      <c r="N92" s="12">
+        <v>100</v>
+      </c>
+      <c r="O92" s="6">
+        <v>43848</v>
+      </c>
+      <c r="P92" s="7">
+        <v>0.21805555555555556</v>
+      </c>
+      <c r="Q92" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="1048576" spans="3:3">
       <c r="C1048576" s="4" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
1209｜EASY｜Convert Binary Number in a Linked List to Integer
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF7852B-3775-4914-864D-6C49C2252D25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629F683B-EAEE-4FA2-9D01-B4F3659FEA0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9930" yWindow="4890" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
+    <workbookView xWindow="6060" yWindow="4890" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="274">
   <si>
     <t>Date</t>
   </si>
@@ -926,10 +926,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Find Numbers with Even Number of Digits</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -947,6 +943,18 @@
   </si>
   <si>
     <t>String｜Greedy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1209</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Convert Binary Number in a Linked List to Integer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Linked List｜Bit Manipulation</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1380,8 +1388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914384AD-4934-744A-8C44-1EF839F36E18}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -5826,8 +5834,8 @@
       <c r="J90" s="12">
         <v>100</v>
       </c>
-      <c r="K90" s="16" t="s">
-        <v>266</v>
+      <c r="K90" s="16">
+        <v>0</v>
       </c>
       <c r="L90" s="12">
         <v>100</v>
@@ -5850,13 +5858,13 @@
     </row>
     <row r="91" spans="1:17">
       <c r="B91" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>94</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E91" s="4" t="s">
         <v>64</v>
@@ -5900,19 +5908,19 @@
     </row>
     <row r="92" spans="1:17">
       <c r="B92" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>94</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E92" s="4" t="s">
         <v>64</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G92" s="4" t="s">
         <v>211</v>
@@ -5945,6 +5953,56 @@
         <v>0.21805555555555556</v>
       </c>
       <c r="Q92" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17">
+      <c r="B93" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="G93" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="H93" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I93" s="16">
+        <v>0</v>
+      </c>
+      <c r="J93" s="12">
+        <v>100</v>
+      </c>
+      <c r="K93" s="16">
+        <v>0</v>
+      </c>
+      <c r="L93" s="12">
+        <v>100</v>
+      </c>
+      <c r="M93" s="22">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="N93" s="12">
+        <v>100</v>
+      </c>
+      <c r="O93" s="6">
+        <v>43848</v>
+      </c>
+      <c r="P93" s="7">
+        <v>0.2298611111111111</v>
+      </c>
+      <c r="Q93" s="20" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1207｜EASY｜Unique Number of Occurrences
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629F683B-EAEE-4FA2-9D01-B4F3659FEA0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A881049-70FF-47C8-BD6D-DC23B6889FCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6060" yWindow="4890" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="278">
   <si>
     <t>Date</t>
   </si>
@@ -955,6 +955,22 @@
   </si>
   <si>
     <t>Linked List｜Bit Manipulation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unique Number of Occurrences</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1207</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hash Table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sort, set.count()</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1388,7 +1404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914384AD-4934-744A-8C44-1EF839F36E18}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
@@ -5973,7 +5989,7 @@
         <v>273</v>
       </c>
       <c r="G93" s="4" t="s">
-        <v>211</v>
+        <v>256</v>
       </c>
       <c r="H93" s="4" t="s">
         <v>13</v>
@@ -6003,6 +6019,56 @@
         <v>0.2298611111111111</v>
       </c>
       <c r="Q93" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17">
+      <c r="B94" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="G94" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="H94" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I94" s="16">
+        <v>0</v>
+      </c>
+      <c r="J94" s="12">
+        <v>100</v>
+      </c>
+      <c r="K94" s="16">
+        <v>4</v>
+      </c>
+      <c r="L94" s="12">
+        <v>74.34</v>
+      </c>
+      <c r="M94" s="22">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="N94" s="12">
+        <v>100</v>
+      </c>
+      <c r="O94" s="6">
+        <v>43848</v>
+      </c>
+      <c r="P94" s="7">
+        <v>0.24166666666666667</v>
+      </c>
+      <c r="Q94" s="20" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1281｜EASY｜Subtract the Product and Sum of Digits of an Integer
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\LeetCode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kzmain/_Repository/👨🏻‍💻LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E65B2B7-0C1A-4E59-8FC9-643881AEDAD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4334515-42AB-7E40-BD45-3E720B19F13F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="4890" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
+    <workbookView xWindow="9560" yWindow="4700" windowWidth="21620" windowHeight="11500" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="283">
   <si>
     <t>Date</t>
   </si>
@@ -984,6 +984,12 @@
   <si>
     <t>sort,compare</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1281</t>
+  </si>
+  <si>
+    <t>Subtract the Product and Sum of Digits of an Integer</t>
   </si>
 </sst>
 </file>
@@ -991,28 +997,28 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="182" formatCode="[$-F400]hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="165" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="166" formatCode="[$-F400]hh:mm:ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1080,7 +1086,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1096,14 +1102,14 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="182" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="182" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="182" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="182" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1420,32 +1426,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914384AD-4934-744A-8C44-1EF839F36E18}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96:XFD96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.875" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="42.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="65.75" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.375" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.625" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="65.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" style="17" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" style="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" style="17" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.125" style="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.875" style="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.375" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.1640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" style="9" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.5" style="27" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.875" style="1"/>
+    <col min="17" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>237</v>
       </c>
@@ -1498,7 +1504,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
         <v>103</v>
       </c>
@@ -1548,7 +1554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>103</v>
       </c>
@@ -1580,7 +1586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>104</v>
       </c>
@@ -1630,7 +1636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
         <v>104</v>
       </c>
@@ -1662,7 +1668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>105</v>
       </c>
@@ -1712,7 +1718,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>106</v>
       </c>
@@ -1762,7 +1768,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>107</v>
       </c>
@@ -1812,7 +1818,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>108</v>
       </c>
@@ -1862,7 +1868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
         <v>109</v>
       </c>
@@ -1912,7 +1918,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
         <v>110</v>
       </c>
@@ -1962,7 +1968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
         <v>111</v>
       </c>
@@ -2012,7 +2018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>112</v>
       </c>
@@ -2062,7 +2068,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
         <v>113</v>
       </c>
@@ -2112,7 +2118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
         <v>114</v>
       </c>
@@ -2162,7 +2168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
         <v>115</v>
       </c>
@@ -2212,7 +2218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:17">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
         <v>115</v>
       </c>
@@ -2262,7 +2268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:17">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
         <v>116</v>
       </c>
@@ -2312,7 +2318,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:17">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="s">
         <v>117</v>
       </c>
@@ -2362,7 +2368,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="2:17">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">
         <v>118</v>
       </c>
@@ -2412,7 +2418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:17">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B21" s="4" t="s">
         <v>119</v>
       </c>
@@ -2462,7 +2468,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:17">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B22" s="4" t="s">
         <v>120</v>
       </c>
@@ -2512,7 +2518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:17">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="s">
         <v>120</v>
       </c>
@@ -2562,7 +2568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:17">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B24" s="4" t="s">
         <v>71</v>
       </c>
@@ -2612,7 +2618,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="2:17">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B25" s="4" t="s">
         <v>121</v>
       </c>
@@ -2662,7 +2668,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="2:17">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B26" s="4" t="s">
         <v>122</v>
       </c>
@@ -2712,7 +2718,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="2:17">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B27" s="4" t="s">
         <v>122</v>
       </c>
@@ -2762,7 +2768,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="2:17">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B28" s="4" t="s">
         <v>123</v>
       </c>
@@ -2812,7 +2818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:17">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B29" s="4" t="s">
         <v>123</v>
       </c>
@@ -2862,7 +2868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:17">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B30" s="4" t="s">
         <v>124</v>
       </c>
@@ -2912,7 +2918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:17">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B31" s="4" t="s">
         <v>125</v>
       </c>
@@ -2962,7 +2968,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="2:17">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B32" s="4" t="s">
         <v>126</v>
       </c>
@@ -3012,7 +3018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:17">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B33" s="4" t="s">
         <v>127</v>
       </c>
@@ -3062,7 +3068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:17">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B34" s="4" t="s">
         <v>128</v>
       </c>
@@ -3112,7 +3118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:17">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B35" s="4" t="s">
         <v>128</v>
       </c>
@@ -3162,7 +3168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:17">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B36" s="4" t="s">
         <v>129</v>
       </c>
@@ -3212,7 +3218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:17">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B37" s="4" t="s">
         <v>129</v>
       </c>
@@ -3262,7 +3268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:17">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B38" s="4" t="s">
         <v>130</v>
       </c>
@@ -3312,7 +3318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:17">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B39" s="4" t="s">
         <v>133</v>
       </c>
@@ -3362,7 +3368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:17">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B40" s="4" t="s">
         <v>137</v>
       </c>
@@ -3412,7 +3418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:17">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B41" s="4" t="s">
         <v>137</v>
       </c>
@@ -3462,7 +3468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:17">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B42" s="4" t="s">
         <v>156</v>
       </c>
@@ -3512,7 +3518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:17">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B43" s="4" t="s">
         <v>156</v>
       </c>
@@ -3562,7 +3568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:17">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B44" s="4" t="s">
         <v>157</v>
       </c>
@@ -3612,7 +3618,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="2:17">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="s">
         <v>158</v>
       </c>
@@ -3662,7 +3668,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="2:17">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B46" s="4" t="s">
         <v>159</v>
       </c>
@@ -3712,7 +3718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:17">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B47" s="4" t="s">
         <v>159</v>
       </c>
@@ -3762,7 +3768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:17">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B48" s="4" t="s">
         <v>160</v>
       </c>
@@ -3812,7 +3818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:17">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B49" s="4" t="s">
         <v>161</v>
       </c>
@@ -3862,7 +3868,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:17">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B50" s="4" t="s">
         <v>164</v>
       </c>
@@ -3912,7 +3918,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="1:17">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B51" s="4" t="s">
         <v>167</v>
       </c>
@@ -3962,7 +3968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:17">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B52" s="4" t="s">
         <v>167</v>
       </c>
@@ -4012,7 +4018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:17">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B53" s="4" t="s">
         <v>167</v>
       </c>
@@ -4062,7 +4068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:17">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B54" s="4" t="s">
         <v>173</v>
       </c>
@@ -4112,7 +4118,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="1:17">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>237</v>
       </c>
@@ -4165,7 +4171,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="1:17">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B56" s="4" t="s">
         <v>177</v>
       </c>
@@ -4215,7 +4221,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:17">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B57" s="4" t="s">
         <v>177</v>
       </c>
@@ -4265,7 +4271,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:17">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B58" s="4" t="s">
         <v>183</v>
       </c>
@@ -4315,7 +4321,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:17">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B59" s="4" t="s">
         <v>185</v>
       </c>
@@ -4365,7 +4371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:17">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B60" s="4" t="s">
         <v>188</v>
       </c>
@@ -4413,7 +4419,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:17">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B61" s="7" t="s">
         <v>188</v>
       </c>
@@ -4445,7 +4451,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="1:17">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B62" s="4" t="s">
         <v>190</v>
       </c>
@@ -4495,7 +4501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:17">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B63" s="4" t="s">
         <v>194</v>
       </c>
@@ -4545,7 +4551,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="1:17">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B64" s="4" t="s">
         <v>194</v>
       </c>
@@ -4595,7 +4601,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="1:17">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B65" s="4" t="s">
         <v>202</v>
       </c>
@@ -4645,7 +4651,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="1:17">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B66" s="7" t="s">
         <v>202</v>
       </c>
@@ -4679,7 +4685,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="1:17">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B67" s="4" t="s">
         <v>203</v>
       </c>
@@ -4729,7 +4735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:17">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B68" s="4" t="s">
         <v>203</v>
       </c>
@@ -4779,7 +4785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:17">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B69" s="4" t="s">
         <v>210</v>
       </c>
@@ -4829,7 +4835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:17">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B70" s="4" t="s">
         <v>212</v>
       </c>
@@ -4879,7 +4885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:17">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B71" s="4" t="s">
         <v>212</v>
       </c>
@@ -4929,7 +4935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:17">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B72" s="4" t="s">
         <v>218</v>
       </c>
@@ -4979,7 +4985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:17">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B73" s="4" t="s">
         <v>220</v>
       </c>
@@ -5029,7 +5035,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="1:17">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B74" s="4" t="s">
         <v>225</v>
       </c>
@@ -5079,7 +5085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:17">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B75" s="4" t="s">
         <v>225</v>
       </c>
@@ -5129,7 +5135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:17">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B76" s="4" t="s">
         <v>225</v>
       </c>
@@ -5179,7 +5185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:17">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B77" s="4" t="s">
         <v>232</v>
       </c>
@@ -5229,7 +5235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:17">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B78" s="4" t="s">
         <v>232</v>
       </c>
@@ -5279,7 +5285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:17">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>237</v>
       </c>
@@ -5332,7 +5338,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="80" spans="1:17">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>237</v>
       </c>
@@ -5385,7 +5391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:17">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>237</v>
       </c>
@@ -5438,7 +5444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:17">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B82" s="4" t="s">
         <v>246</v>
       </c>
@@ -5488,7 +5494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:17">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B83" s="4" t="s">
         <v>246</v>
       </c>
@@ -5538,7 +5544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:17">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B84" s="4" t="s">
         <v>249</v>
       </c>
@@ -5588,7 +5594,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="1:17">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B85" s="4" t="s">
         <v>254</v>
       </c>
@@ -5638,7 +5644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:17">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B86" s="4" t="s">
         <v>254</v>
       </c>
@@ -5688,7 +5694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:17">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B87" s="4" t="s">
         <v>258</v>
       </c>
@@ -5738,7 +5744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:17">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B88" s="4" t="s">
         <v>258</v>
       </c>
@@ -5788,7 +5794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:17">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B89" s="4" t="s">
         <v>262</v>
       </c>
@@ -5838,7 +5844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:17">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B90" s="4" t="s">
         <v>264</v>
       </c>
@@ -5888,7 +5894,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="91" spans="1:17">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B91" s="4" t="s">
         <v>267</v>
       </c>
@@ -5938,7 +5944,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="92" spans="1:17">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B92" s="4" t="s">
         <v>269</v>
       </c>
@@ -5988,7 +5994,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="93" spans="1:17">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B93" s="4" t="s">
         <v>271</v>
       </c>
@@ -6038,7 +6044,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="94" spans="1:17">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B94" s="4" t="s">
         <v>275</v>
       </c>
@@ -6088,7 +6094,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="95" spans="1:17">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B95" s="4" t="s">
         <v>278</v>
       </c>
@@ -6138,7 +6144,57 @@
         <v>32</v>
       </c>
     </row>
-    <row r="1048576" spans="3:3">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B96" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G96" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="H96" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I96" s="15">
+        <v>0</v>
+      </c>
+      <c r="J96" s="11">
+        <v>100</v>
+      </c>
+      <c r="K96" s="15">
+        <v>0</v>
+      </c>
+      <c r="L96" s="11">
+        <v>100</v>
+      </c>
+      <c r="M96" s="21">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="N96" s="11">
+        <v>100</v>
+      </c>
+      <c r="O96" s="6">
+        <v>43848</v>
+      </c>
+      <c r="P96" s="25">
+        <v>0.98472222222222217</v>
+      </c>
+      <c r="Q96" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="1048576" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C1048576" s="4" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
0905｜EASY｜Sort Array By Parity
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kzmain/_Repository/👨🏻‍💻LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4334515-42AB-7E40-BD45-3E720B19F13F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABDA512E-9EB7-7E41-936D-F9C0A5CED8D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9560" yWindow="4700" windowWidth="21620" windowHeight="11500" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="287">
   <si>
     <t>Date</t>
   </si>
@@ -990,6 +990,18 @@
   </si>
   <si>
     <t>Subtract the Product and Sum of Digits of an Integer</t>
+  </si>
+  <si>
+    <t>0905</t>
+  </si>
+  <si>
+    <t>Sort Array By Parity</t>
+  </si>
+  <si>
+    <t>注意vectorbound</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -1426,8 +1438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914384AD-4934-744A-8C44-1EF839F36E18}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96:XFD96"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6194,6 +6206,56 @@
         <v>32</v>
       </c>
     </row>
+    <row r="97" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B97" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G97" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="H97" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="I97" s="15">
+        <v>28</v>
+      </c>
+      <c r="J97" s="11">
+        <v>76.180000000000007</v>
+      </c>
+      <c r="K97" s="15">
+        <v>28</v>
+      </c>
+      <c r="L97" s="11">
+        <v>76.180000000000007</v>
+      </c>
+      <c r="M97" s="21">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="N97" s="11">
+        <v>72.41</v>
+      </c>
+      <c r="O97" s="6">
+        <v>43848</v>
+      </c>
+      <c r="P97" s="25">
+        <v>2.9166666666666664E-2</v>
+      </c>
+      <c r="Q97" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C1048576" s="4" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
0720｜EASY｜Longest Word in Dictionary
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kzmain/_Repository/👨🏻‍💻LeetCode/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2713A57-AC6F-E14A-B0CC-FB91A5565B86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF383874-A9FF-4B6F-8FB0-71281DEF6BE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9560" yWindow="4700" windowWidth="21620" windowHeight="11500" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
+    <workbookView xWindow="5040" yWindow="2430" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="296">
   <si>
     <t>Date</t>
   </si>
@@ -1017,6 +1017,22 @@
   </si>
   <si>
     <t>sort以后，取唯一</t>
+  </si>
+  <si>
+    <t>可能缺少前面的部分，多个长度的string可能有相同的前缀</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0720</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Longest Word in Dictionary</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hash Table｜Trie</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1024,28 +1040,28 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="165" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="166" formatCode="[$-F400]hh:mm:ss"/>
+    <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="178" formatCode="[$-F400]hh:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1113,7 +1129,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1129,14 +1145,14 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1454,31 +1470,31 @@
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A87" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92"/>
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="4.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.125" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.83203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.875" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.125" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="42.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="65.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="65.625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.375" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.625" style="17" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" style="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" style="17" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.1640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.125" style="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.875" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.375" style="9" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.5" style="27" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="1"/>
+    <col min="17" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17">
       <c r="A1" s="2" t="s">
         <v>237</v>
       </c>
@@ -1531,7 +1547,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17">
       <c r="B2" s="4" t="s">
         <v>103</v>
       </c>
@@ -1581,7 +1597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17">
       <c r="B3" s="7" t="s">
         <v>103</v>
       </c>
@@ -1613,7 +1629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17">
       <c r="B4" s="4" t="s">
         <v>104</v>
       </c>
@@ -1663,7 +1679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17">
       <c r="B5" s="7" t="s">
         <v>104</v>
       </c>
@@ -1695,7 +1711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17">
       <c r="B6" s="4" t="s">
         <v>105</v>
       </c>
@@ -1745,7 +1761,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17">
       <c r="B7" s="4" t="s">
         <v>106</v>
       </c>
@@ -1795,7 +1811,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17">
       <c r="B8" s="4" t="s">
         <v>107</v>
       </c>
@@ -1845,7 +1861,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17">
       <c r="B9" s="4" t="s">
         <v>108</v>
       </c>
@@ -1895,7 +1911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17">
       <c r="B10" s="4" t="s">
         <v>109</v>
       </c>
@@ -1945,7 +1961,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17">
       <c r="B11" s="4" t="s">
         <v>110</v>
       </c>
@@ -1995,7 +2011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17">
       <c r="B12" s="4" t="s">
         <v>111</v>
       </c>
@@ -2045,7 +2061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17">
       <c r="B13" s="4" t="s">
         <v>112</v>
       </c>
@@ -2095,7 +2111,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17">
       <c r="B14" s="4" t="s">
         <v>113</v>
       </c>
@@ -2145,7 +2161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17">
       <c r="B15" s="4" t="s">
         <v>114</v>
       </c>
@@ -2195,7 +2211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17">
       <c r="B16" s="4" t="s">
         <v>115</v>
       </c>
@@ -2245,7 +2261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:17">
       <c r="B17" s="4" t="s">
         <v>115</v>
       </c>
@@ -2295,7 +2311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:17">
       <c r="B18" s="4" t="s">
         <v>116</v>
       </c>
@@ -2345,7 +2361,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:17">
       <c r="B19" s="4" t="s">
         <v>117</v>
       </c>
@@ -2395,7 +2411,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:17">
       <c r="B20" s="4" t="s">
         <v>118</v>
       </c>
@@ -2445,7 +2461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:17">
       <c r="B21" s="4" t="s">
         <v>119</v>
       </c>
@@ -2495,7 +2511,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:17">
       <c r="B22" s="4" t="s">
         <v>120</v>
       </c>
@@ -2545,7 +2561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:17">
       <c r="B23" s="4" t="s">
         <v>120</v>
       </c>
@@ -2595,7 +2611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:17">
       <c r="B24" s="4" t="s">
         <v>71</v>
       </c>
@@ -2645,7 +2661,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:17">
       <c r="B25" s="4" t="s">
         <v>121</v>
       </c>
@@ -2695,7 +2711,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:17">
       <c r="B26" s="4" t="s">
         <v>122</v>
       </c>
@@ -2745,7 +2761,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:17">
       <c r="B27" s="4" t="s">
         <v>122</v>
       </c>
@@ -2795,7 +2811,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:17">
       <c r="B28" s="4" t="s">
         <v>123</v>
       </c>
@@ -2845,7 +2861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:17">
       <c r="B29" s="4" t="s">
         <v>123</v>
       </c>
@@ -2895,7 +2911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:17">
       <c r="B30" s="4" t="s">
         <v>124</v>
       </c>
@@ -2945,7 +2961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:17">
       <c r="B31" s="4" t="s">
         <v>125</v>
       </c>
@@ -2995,7 +3011,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:17">
       <c r="B32" s="4" t="s">
         <v>126</v>
       </c>
@@ -3045,7 +3061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:17">
       <c r="B33" s="4" t="s">
         <v>127</v>
       </c>
@@ -3095,7 +3111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:17">
       <c r="B34" s="4" t="s">
         <v>128</v>
       </c>
@@ -3145,7 +3161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:17">
       <c r="B35" s="4" t="s">
         <v>128</v>
       </c>
@@ -3195,7 +3211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:17">
       <c r="B36" s="4" t="s">
         <v>129</v>
       </c>
@@ -3245,7 +3261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:17">
       <c r="B37" s="4" t="s">
         <v>129</v>
       </c>
@@ -3295,7 +3311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:17">
       <c r="B38" s="4" t="s">
         <v>130</v>
       </c>
@@ -3345,7 +3361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:17">
       <c r="B39" s="4" t="s">
         <v>133</v>
       </c>
@@ -3395,7 +3411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:17">
       <c r="B40" s="4" t="s">
         <v>137</v>
       </c>
@@ -3445,7 +3461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:17">
       <c r="B41" s="4" t="s">
         <v>137</v>
       </c>
@@ -3495,7 +3511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:17">
       <c r="B42" s="4" t="s">
         <v>156</v>
       </c>
@@ -3545,7 +3561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:17">
       <c r="B43" s="4" t="s">
         <v>156</v>
       </c>
@@ -3595,7 +3611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:17">
       <c r="B44" s="4" t="s">
         <v>157</v>
       </c>
@@ -3645,7 +3661,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:17">
       <c r="B45" s="4" t="s">
         <v>158</v>
       </c>
@@ -3695,7 +3711,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:17">
       <c r="B46" s="4" t="s">
         <v>159</v>
       </c>
@@ -3745,7 +3761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:17">
       <c r="B47" s="4" t="s">
         <v>159</v>
       </c>
@@ -3795,7 +3811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:17">
       <c r="B48" s="4" t="s">
         <v>160</v>
       </c>
@@ -3845,7 +3861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17">
       <c r="B49" s="4" t="s">
         <v>161</v>
       </c>
@@ -3895,7 +3911,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17">
       <c r="B50" s="4" t="s">
         <v>164</v>
       </c>
@@ -3945,7 +3961,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17">
       <c r="B51" s="4" t="s">
         <v>167</v>
       </c>
@@ -3995,7 +4011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17">
       <c r="B52" s="4" t="s">
         <v>167</v>
       </c>
@@ -4045,7 +4061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17">
       <c r="B53" s="4" t="s">
         <v>167</v>
       </c>
@@ -4095,7 +4111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17">
       <c r="B54" s="4" t="s">
         <v>173</v>
       </c>
@@ -4145,7 +4161,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17">
       <c r="A55" s="1" t="s">
         <v>237</v>
       </c>
@@ -4198,7 +4214,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17">
       <c r="B56" s="4" t="s">
         <v>177</v>
       </c>
@@ -4248,7 +4264,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17">
       <c r="B57" s="4" t="s">
         <v>177</v>
       </c>
@@ -4298,7 +4314,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17">
       <c r="B58" s="4" t="s">
         <v>183</v>
       </c>
@@ -4348,7 +4364,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17">
       <c r="B59" s="4" t="s">
         <v>185</v>
       </c>
@@ -4398,7 +4414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17">
       <c r="B60" s="4" t="s">
         <v>188</v>
       </c>
@@ -4446,7 +4462,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17">
       <c r="B61" s="7" t="s">
         <v>188</v>
       </c>
@@ -4478,7 +4494,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:17">
       <c r="B62" s="4" t="s">
         <v>190</v>
       </c>
@@ -4528,7 +4544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17">
       <c r="B63" s="4" t="s">
         <v>194</v>
       </c>
@@ -4578,7 +4594,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:17">
       <c r="B64" s="4" t="s">
         <v>194</v>
       </c>
@@ -4628,7 +4644,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17">
       <c r="B65" s="4" t="s">
         <v>202</v>
       </c>
@@ -4678,7 +4694,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:17">
       <c r="B66" s="7" t="s">
         <v>202</v>
       </c>
@@ -4712,7 +4728,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:17">
       <c r="B67" s="4" t="s">
         <v>203</v>
       </c>
@@ -4762,7 +4778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17">
       <c r="B68" s="4" t="s">
         <v>203</v>
       </c>
@@ -4812,7 +4828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:17">
       <c r="B69" s="4" t="s">
         <v>210</v>
       </c>
@@ -4862,7 +4878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:17">
       <c r="B70" s="4" t="s">
         <v>212</v>
       </c>
@@ -4912,7 +4928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:17">
       <c r="B71" s="4" t="s">
         <v>212</v>
       </c>
@@ -4962,7 +4978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:17">
       <c r="B72" s="4" t="s">
         <v>218</v>
       </c>
@@ -5012,7 +5028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:17">
       <c r="B73" s="4" t="s">
         <v>220</v>
       </c>
@@ -5062,7 +5078,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:17">
       <c r="B74" s="4" t="s">
         <v>225</v>
       </c>
@@ -5112,7 +5128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:17">
       <c r="B75" s="4" t="s">
         <v>225</v>
       </c>
@@ -5162,7 +5178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:17">
       <c r="B76" s="4" t="s">
         <v>225</v>
       </c>
@@ -5212,7 +5228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:17">
       <c r="B77" s="4" t="s">
         <v>232</v>
       </c>
@@ -5262,7 +5278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:17">
       <c r="B78" s="4" t="s">
         <v>232</v>
       </c>
@@ -5312,7 +5328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:17">
       <c r="A79" s="1" t="s">
         <v>237</v>
       </c>
@@ -5365,7 +5381,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:17">
       <c r="A80" s="1" t="s">
         <v>237</v>
       </c>
@@ -5418,7 +5434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:17">
       <c r="A81" s="1" t="s">
         <v>237</v>
       </c>
@@ -5471,7 +5487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:17">
       <c r="B82" s="4" t="s">
         <v>246</v>
       </c>
@@ -5521,7 +5537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:17">
       <c r="B83" s="4" t="s">
         <v>246</v>
       </c>
@@ -5571,7 +5587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:17">
       <c r="B84" s="4" t="s">
         <v>249</v>
       </c>
@@ -5621,7 +5637,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:17">
       <c r="B85" s="4" t="s">
         <v>254</v>
       </c>
@@ -5671,7 +5687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:17">
       <c r="B86" s="4" t="s">
         <v>254</v>
       </c>
@@ -5721,7 +5737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:17">
       <c r="B87" s="4" t="s">
         <v>258</v>
       </c>
@@ -5771,7 +5787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:17">
       <c r="B88" s="4" t="s">
         <v>258</v>
       </c>
@@ -5821,7 +5837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:17">
       <c r="B89" s="4" t="s">
         <v>262</v>
       </c>
@@ -5871,7 +5887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:17">
       <c r="B90" s="4" t="s">
         <v>264</v>
       </c>
@@ -5921,7 +5937,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:17">
       <c r="B91" s="4" t="s">
         <v>267</v>
       </c>
@@ -5971,7 +5987,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:17">
       <c r="B92" s="4" t="s">
         <v>269</v>
       </c>
@@ -6021,7 +6037,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:17">
       <c r="B93" s="4" t="s">
         <v>271</v>
       </c>
@@ -6071,7 +6087,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:17">
       <c r="B94" s="4" t="s">
         <v>275</v>
       </c>
@@ -6121,7 +6137,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:17">
       <c r="B95" s="4" t="s">
         <v>278</v>
       </c>
@@ -6171,7 +6187,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:17">
       <c r="B96" s="4" t="s">
         <v>281</v>
       </c>
@@ -6221,7 +6237,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="97" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:17">
       <c r="B97" s="4" t="s">
         <v>283</v>
       </c>
@@ -6271,7 +6287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:17">
       <c r="B98" s="4" t="s">
         <v>286</v>
       </c>
@@ -6319,7 +6335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:17">
       <c r="B99" s="4" t="s">
         <v>288</v>
       </c>
@@ -6369,7 +6385,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="100" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:17">
       <c r="B100" s="4" t="s">
         <v>288</v>
       </c>
@@ -6419,7 +6435,57 @@
         <v>32</v>
       </c>
     </row>
-    <row r="1048576" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:17">
+      <c r="B101" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="G101" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="H101" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I101" s="15">
+        <v>76</v>
+      </c>
+      <c r="J101" s="11">
+        <v>31.51</v>
+      </c>
+      <c r="K101" s="15">
+        <v>76</v>
+      </c>
+      <c r="L101" s="11">
+        <v>31.51</v>
+      </c>
+      <c r="M101" s="21">
+        <v>18.2</v>
+      </c>
+      <c r="N101" s="11">
+        <v>100</v>
+      </c>
+      <c r="O101" s="6">
+        <v>43850</v>
+      </c>
+      <c r="P101" s="25">
+        <v>2.5694444444444447E-2</v>
+      </c>
+      <c r="Q101" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1048576" spans="3:3">
       <c r="C1048576" s="4" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
1299｜EASY｜Replace Elements with Greatest Element on Right Side
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CB9618-661F-4740-AB33-CD68A8D5E888}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE048F6-16C9-4C2F-8159-B48D77D6233B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="2430" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
+    <workbookView xWindow="7290" yWindow="3930" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="306">
   <si>
     <t>Date</t>
   </si>
@@ -1056,6 +1056,22 @@
   </si>
   <si>
     <t>Maximum 69 Number</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>找到从左到右最大的数字，比较temp和replace，赋值太多次会影响</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Replace Elements with Greatest Element on Right Side</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1299</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>push -1到最后的vect，右边比左边大的时候，左边用右边替换</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1493,8 +1509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914384AD-4934-744A-8C44-1EF839F36E18}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -6662,6 +6678,106 @@
         <v>32</v>
       </c>
     </row>
+    <row r="105" spans="1:17">
+      <c r="B105" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F105" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G105" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="H105" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I105" s="15">
+        <v>52</v>
+      </c>
+      <c r="J105" s="11">
+        <v>76.45</v>
+      </c>
+      <c r="K105" s="15">
+        <v>52</v>
+      </c>
+      <c r="L105" s="11">
+        <v>76.45</v>
+      </c>
+      <c r="M105" s="21">
+        <v>10.6</v>
+      </c>
+      <c r="N105" s="11">
+        <v>100</v>
+      </c>
+      <c r="O105" s="6">
+        <v>43850</v>
+      </c>
+      <c r="P105" s="25">
+        <v>0.11041666666666666</v>
+      </c>
+      <c r="Q105" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17">
+      <c r="B106" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F106" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G106" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="H106" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I106" s="15">
+        <v>48</v>
+      </c>
+      <c r="J106" s="11">
+        <v>93.33</v>
+      </c>
+      <c r="K106" s="15">
+        <v>52</v>
+      </c>
+      <c r="L106" s="11">
+        <v>76.45</v>
+      </c>
+      <c r="M106" s="21">
+        <v>11</v>
+      </c>
+      <c r="N106" s="11">
+        <v>100</v>
+      </c>
+      <c r="O106" s="6">
+        <v>43850</v>
+      </c>
+      <c r="P106" s="25">
+        <v>0.11041666666666666</v>
+      </c>
+      <c r="Q106" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="1048576" spans="3:3">
       <c r="C1048576" s="4" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
1287｜EASY｜Element Appearing More Than 25% In Sorted Array
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE048F6-16C9-4C2F-8159-B48D77D6233B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67ABCEA1-4FAF-4433-9843-24017322BCCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7290" yWindow="3930" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
+    <workbookView xWindow="8160" yWindow="3735" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="310">
   <si>
     <t>Date</t>
   </si>
@@ -1072,6 +1072,22 @@
   </si>
   <si>
     <t>push -1到最后的vect，右边比左边大的时候，左边用右边替换</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Element Appearing More Than 25% In Sorted Array</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1287</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>用map一个个累加找到最大值</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>在1/4，1/2，3/4的位置截取</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1509,8 +1525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914384AD-4934-744A-8C44-1EF839F36E18}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103"/>
+    <sheetView tabSelected="1" topLeftCell="G106" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J108" sqref="J108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -6778,6 +6794,106 @@
         <v>32</v>
       </c>
     </row>
+    <row r="107" spans="1:17">
+      <c r="B107" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="E107" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F107" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G107" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="H107" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I107" s="15">
+        <v>20</v>
+      </c>
+      <c r="J107" s="11">
+        <v>44.55</v>
+      </c>
+      <c r="K107" s="15">
+        <v>24</v>
+      </c>
+      <c r="L107" s="11">
+        <v>22.16</v>
+      </c>
+      <c r="M107" s="21">
+        <v>10.4</v>
+      </c>
+      <c r="N107" s="11">
+        <v>100</v>
+      </c>
+      <c r="O107" s="6">
+        <v>43850</v>
+      </c>
+      <c r="P107" s="25">
+        <v>0.15833333333333333</v>
+      </c>
+      <c r="Q107" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17">
+      <c r="B108" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F108" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G108" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="H108" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I108" s="15">
+        <v>16</v>
+      </c>
+      <c r="J108" s="11">
+        <v>85.8</v>
+      </c>
+      <c r="K108" s="15">
+        <v>16</v>
+      </c>
+      <c r="L108" s="11">
+        <v>85.8</v>
+      </c>
+      <c r="M108" s="21">
+        <v>9.4</v>
+      </c>
+      <c r="N108" s="11">
+        <v>100</v>
+      </c>
+      <c r="O108" s="6">
+        <v>43850</v>
+      </c>
+      <c r="P108" s="25">
+        <v>0.15833333333333333</v>
+      </c>
+      <c r="Q108" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="1048576" spans="3:3">
       <c r="C1048576" s="4" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
1266｜EASY｜Minimum Time Visiting All Points
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67ABCEA1-4FAF-4433-9843-24017322BCCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C456B4-A6A1-4328-BE01-4E46A0E36B11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8160" yWindow="3735" windowWidth="21615" windowHeight="11505" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
+    <workbookView xWindow="5265" yWindow="3300" windowWidth="21615" windowHeight="11355" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="315">
   <si>
     <t>Date</t>
   </si>
@@ -1088,6 +1088,26 @@
   </si>
   <si>
     <t>在1/4，1/2，3/4的位置截取</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Minimum Time Visiting All Points</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1266</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Array｜Geometry</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>计算距离，point2计算新（x）（y）的位置，然后加减</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>判断上下左右直接加减</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1525,8 +1545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914384AD-4934-744A-8C44-1EF839F36E18}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G106" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J108" sqref="J108"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -6894,6 +6914,112 @@
         <v>32</v>
       </c>
     </row>
+    <row r="109" spans="1:17">
+      <c r="A109" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E109" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F109" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="G109" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="H109" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I109" s="15">
+        <v>12</v>
+      </c>
+      <c r="J109" s="11">
+        <v>48.03</v>
+      </c>
+      <c r="K109" s="15">
+        <v>12</v>
+      </c>
+      <c r="L109" s="11">
+        <v>48.03</v>
+      </c>
+      <c r="M109" s="21">
+        <v>10.1</v>
+      </c>
+      <c r="N109" s="11">
+        <v>100</v>
+      </c>
+      <c r="O109" s="6">
+        <v>43850</v>
+      </c>
+      <c r="P109" s="25">
+        <v>0.7006944444444444</v>
+      </c>
+      <c r="Q109" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17">
+      <c r="A110" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D110" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E110" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F110" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="G110" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="H110" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I110" s="15">
+        <v>4</v>
+      </c>
+      <c r="J110" s="11">
+        <v>99.32</v>
+      </c>
+      <c r="K110" s="15">
+        <v>8</v>
+      </c>
+      <c r="L110" s="11">
+        <v>89.23</v>
+      </c>
+      <c r="M110" s="21">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="N110" s="11">
+        <v>100</v>
+      </c>
+      <c r="O110" s="6">
+        <v>43850</v>
+      </c>
+      <c r="P110" s="25">
+        <v>0.7006944444444444</v>
+      </c>
+      <c r="Q110" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="1048576" spans="3:3">
       <c r="C1048576" s="4" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
0448｜EASY｜Find All Numbers Disappeared in an Array
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9E285E-A85C-4336-8386-856BABF61C7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0A5DAE-707C-4529-B0F1-9DF1E0A1BE92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5265" yWindow="3300" windowWidth="21615" windowHeight="11355" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
+    <workbookView xWindow="5505" yWindow="3885" windowWidth="21615" windowHeight="11355" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="326">
   <si>
     <t>Date</t>
   </si>
@@ -1136,6 +1136,22 @@
   </si>
   <si>
     <t>计算出现0的次数从最后一位iterate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Find All Numbers Disappeared in an Array</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0448</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sort了以后一个个找谁不存在</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>用-当时的值代表i这个位置是有数字的，用作hash，很有用</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1573,8 +1589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914384AD-4934-744A-8C44-1EF839F36E18}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D109" sqref="D109"/>
+    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A127" sqref="A127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -6943,9 +6959,6 @@
       </c>
     </row>
     <row r="109" spans="1:17">
-      <c r="A109" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="B109" s="4" t="s">
         <v>311</v>
       </c>
@@ -7102,9 +7115,6 @@
       </c>
     </row>
     <row r="112" spans="1:17">
-      <c r="A112" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="B112" s="4" t="s">
         <v>318</v>
       </c>
@@ -7205,6 +7215,109 @@
       </c>
       <c r="Q113" s="19" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:17">
+      <c r="B114" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D114" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="E114" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F114" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G114" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="H114" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I114" s="15">
+        <v>140</v>
+      </c>
+      <c r="J114" s="11">
+        <v>20.59</v>
+      </c>
+      <c r="K114" s="15">
+        <v>140</v>
+      </c>
+      <c r="L114" s="11">
+        <v>20.59</v>
+      </c>
+      <c r="M114" s="21">
+        <v>14.9</v>
+      </c>
+      <c r="N114" s="11">
+        <v>70</v>
+      </c>
+      <c r="O114" s="6">
+        <v>43850</v>
+      </c>
+      <c r="P114" s="25">
+        <v>5.2777777777777778E-2</v>
+      </c>
+      <c r="Q114" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="115" spans="1:17">
+      <c r="A115" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D115" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="E115" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F115" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G115" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="H115" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I115" s="16">
+        <v>112</v>
+      </c>
+      <c r="J115" s="12">
+        <v>90.66</v>
+      </c>
+      <c r="K115" s="16">
+        <v>14.9</v>
+      </c>
+      <c r="L115" s="12">
+        <v>93.33</v>
+      </c>
+      <c r="M115" s="22">
+        <v>14.9</v>
+      </c>
+      <c r="N115" s="12">
+        <v>93.33</v>
+      </c>
+      <c r="O115" s="8">
+        <v>43850</v>
+      </c>
+      <c r="P115" s="26">
+        <v>5.2777777777777778E-2</v>
+      </c>
+      <c r="Q115" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="1048576" spans="3:3">

</xml_diff>

<commit_message>
1103｜EASY｜Distribute Candies to People
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0A5DAE-707C-4529-B0F1-9DF1E0A1BE92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB02F675-61B3-403E-9255-24C1DFBD8083}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5505" yWindow="3885" windowWidth="21615" windowHeight="11355" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="328">
   <si>
     <t>Date</t>
   </si>
@@ -1152,6 +1152,14 @@
   </si>
   <si>
     <t>用-当时的值代表i这个位置是有数字的，用作hash，很有用</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1103</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Distribute Candies to People</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1242,7 +1250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1273,6 +1281,7 @@
     <xf numFmtId="178" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="178" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="178" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1589,8 +1598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914384AD-4934-744A-8C44-1EF839F36E18}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A127" sqref="A127"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -7310,13 +7319,63 @@
       <c r="N115" s="12">
         <v>93.33</v>
       </c>
-      <c r="O115" s="8">
+      <c r="O115" s="28">
         <v>43850</v>
       </c>
       <c r="P115" s="26">
         <v>5.2777777777777778E-2</v>
       </c>
       <c r="Q115" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="116" spans="1:17">
+      <c r="B116" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D116" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="E116" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F116" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G116" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H116" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I116" s="15">
+        <v>0</v>
+      </c>
+      <c r="J116" s="11">
+        <v>100</v>
+      </c>
+      <c r="K116" s="15">
+        <v>4</v>
+      </c>
+      <c r="L116" s="11">
+        <v>64.89</v>
+      </c>
+      <c r="M116" s="21">
+        <v>8.6</v>
+      </c>
+      <c r="N116" s="11">
+        <v>100</v>
+      </c>
+      <c r="O116" s="6">
+        <v>43850</v>
+      </c>
+      <c r="P116" s="25">
+        <v>0.1125</v>
+      </c>
+      <c r="Q116" s="19" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1108｜EASY｜Defanging an IP Address
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB02F675-61B3-403E-9255-24C1DFBD8083}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4788CE0E-8D33-436B-AD8A-59EE8F978C60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5505" yWindow="3885" windowWidth="21615" windowHeight="11355" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="330">
   <si>
     <t>Date</t>
   </si>
@@ -1160,6 +1160,14 @@
   </si>
   <si>
     <t>Distribute Candies to People</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1108</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Defanging an IP Address</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1599,7 +1607,7 @@
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A103" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E111" sqref="E111"/>
+      <selection activeCell="A117" sqref="A117:XFD117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -1619,7 +1627,7 @@
     <col min="13" max="13" width="13.125" style="23" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.875" style="13" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.375" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.5" style="27" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.25" style="27" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
@@ -7379,6 +7387,56 @@
         <v>28</v>
       </c>
     </row>
+    <row r="117" spans="1:17">
+      <c r="B117" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D117" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="E117" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F117" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="G117" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="H117" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I117" s="15">
+        <v>0</v>
+      </c>
+      <c r="J117" s="11">
+        <v>100</v>
+      </c>
+      <c r="K117" s="15">
+        <v>0</v>
+      </c>
+      <c r="L117" s="11">
+        <v>100</v>
+      </c>
+      <c r="M117" s="21">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="N117" s="11">
+        <v>100</v>
+      </c>
+      <c r="O117" s="6">
+        <v>43850</v>
+      </c>
+      <c r="P117" s="25">
+        <v>0.12083333333333333</v>
+      </c>
+      <c r="Q117" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="1048576" spans="3:3">
       <c r="C1048576" s="4" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
1047｜EASY｜Remove All Adjacent Duplicates In String
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\LeetCode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kzmain/_Repository/👨🏻‍💻LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04076E0B-45F7-440A-B4C0-5A0ECA65ECA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D4B837-EDD9-6447-8774-DC00B2DD803A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5505" yWindow="3885" windowWidth="21615" windowHeight="11355" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
+    <workbookView xWindow="8300" yWindow="2820" windowWidth="21620" windowHeight="11360" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="338">
   <si>
     <t>Date</t>
   </si>
@@ -1185,6 +1185,18 @@
   <si>
     <t>1122</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1047</t>
+  </si>
+  <si>
+    <t>Remove All Adjacent Duplicates In String</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>string -&gt;  char vector -&gt; Simulate stack</t>
   </si>
 </sst>
 </file>
@@ -1192,28 +1204,28 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="178" formatCode="[$-F400]hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="165" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="166" formatCode="[$-F400]hh:mm:ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1281,7 +1293,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1297,15 +1309,15 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1622,32 +1634,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914384AD-4934-744A-8C44-1EF839F36E18}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B103" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B119" sqref="A119:XFD119"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.875" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="42.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="65.625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.375" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.625" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="65.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" style="17" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" style="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" style="17" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.125" style="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.875" style="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.375" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.25" style="27" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.875" style="1"/>
+    <col min="13" max="13" width="13.1640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.1640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>237</v>
       </c>
@@ -1700,7 +1712,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
         <v>103</v>
       </c>
@@ -1750,7 +1762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>103</v>
       </c>
@@ -1782,7 +1794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>104</v>
       </c>
@@ -1832,7 +1844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
         <v>104</v>
       </c>
@@ -1864,7 +1876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>105</v>
       </c>
@@ -1914,7 +1926,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>106</v>
       </c>
@@ -1964,7 +1976,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>107</v>
       </c>
@@ -2014,7 +2026,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>108</v>
       </c>
@@ -2064,7 +2076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
         <v>109</v>
       </c>
@@ -2114,7 +2126,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
         <v>110</v>
       </c>
@@ -2164,7 +2176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
         <v>111</v>
       </c>
@@ -2214,7 +2226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>112</v>
       </c>
@@ -2264,7 +2276,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
         <v>113</v>
       </c>
@@ -2314,7 +2326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
         <v>114</v>
       </c>
@@ -2364,7 +2376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
         <v>115</v>
       </c>
@@ -2414,7 +2426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:17">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
         <v>115</v>
       </c>
@@ -2464,7 +2476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:17">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
         <v>116</v>
       </c>
@@ -2514,7 +2526,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:17">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="s">
         <v>117</v>
       </c>
@@ -2564,7 +2576,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="2:17">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">
         <v>118</v>
       </c>
@@ -2614,7 +2626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:17">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B21" s="4" t="s">
         <v>119</v>
       </c>
@@ -2664,7 +2676,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:17">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B22" s="4" t="s">
         <v>120</v>
       </c>
@@ -2714,7 +2726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:17">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="s">
         <v>120</v>
       </c>
@@ -2764,7 +2776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:17">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B24" s="4" t="s">
         <v>71</v>
       </c>
@@ -2814,7 +2826,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="2:17">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B25" s="4" t="s">
         <v>121</v>
       </c>
@@ -2864,7 +2876,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="2:17">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B26" s="4" t="s">
         <v>122</v>
       </c>
@@ -2914,7 +2926,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="2:17">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B27" s="4" t="s">
         <v>122</v>
       </c>
@@ -2964,7 +2976,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="2:17">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B28" s="4" t="s">
         <v>123</v>
       </c>
@@ -3014,7 +3026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:17">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B29" s="4" t="s">
         <v>123</v>
       </c>
@@ -3064,7 +3076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:17">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B30" s="4" t="s">
         <v>124</v>
       </c>
@@ -3114,7 +3126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:17">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B31" s="4" t="s">
         <v>125</v>
       </c>
@@ -3164,7 +3176,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="2:17">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B32" s="4" t="s">
         <v>126</v>
       </c>
@@ -3214,7 +3226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:17">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B33" s="4" t="s">
         <v>127</v>
       </c>
@@ -3264,7 +3276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:17">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B34" s="4" t="s">
         <v>128</v>
       </c>
@@ -3314,7 +3326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:17">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B35" s="4" t="s">
         <v>128</v>
       </c>
@@ -3364,7 +3376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:17">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B36" s="4" t="s">
         <v>129</v>
       </c>
@@ -3414,7 +3426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:17">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B37" s="4" t="s">
         <v>129</v>
       </c>
@@ -3464,7 +3476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:17">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B38" s="4" t="s">
         <v>130</v>
       </c>
@@ -3514,7 +3526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:17">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B39" s="4" t="s">
         <v>133</v>
       </c>
@@ -3564,7 +3576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:17">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B40" s="4" t="s">
         <v>137</v>
       </c>
@@ -3614,7 +3626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:17">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B41" s="4" t="s">
         <v>137</v>
       </c>
@@ -3664,7 +3676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:17">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B42" s="4" t="s">
         <v>156</v>
       </c>
@@ -3714,7 +3726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:17">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B43" s="4" t="s">
         <v>156</v>
       </c>
@@ -3764,7 +3776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:17">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B44" s="4" t="s">
         <v>157</v>
       </c>
@@ -3814,7 +3826,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="2:17">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="s">
         <v>158</v>
       </c>
@@ -3864,7 +3876,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="2:17">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B46" s="4" t="s">
         <v>159</v>
       </c>
@@ -3914,7 +3926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:17">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B47" s="4" t="s">
         <v>159</v>
       </c>
@@ -3964,7 +3976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:17">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B48" s="4" t="s">
         <v>160</v>
       </c>
@@ -4014,7 +4026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:17">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B49" s="4" t="s">
         <v>161</v>
       </c>
@@ -4064,7 +4076,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:17">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B50" s="4" t="s">
         <v>164</v>
       </c>
@@ -4114,7 +4126,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="1:17">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B51" s="4" t="s">
         <v>167</v>
       </c>
@@ -4164,7 +4176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:17">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B52" s="4" t="s">
         <v>167</v>
       </c>
@@ -4214,7 +4226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:17">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B53" s="4" t="s">
         <v>167</v>
       </c>
@@ -4264,7 +4276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:17">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B54" s="4" t="s">
         <v>173</v>
       </c>
@@ -4314,7 +4326,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="1:17">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>237</v>
       </c>
@@ -4367,7 +4379,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="1:17">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B56" s="4" t="s">
         <v>177</v>
       </c>
@@ -4417,7 +4429,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:17">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B57" s="4" t="s">
         <v>177</v>
       </c>
@@ -4467,7 +4479,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:17">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B58" s="4" t="s">
         <v>183</v>
       </c>
@@ -4517,7 +4529,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:17">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B59" s="4" t="s">
         <v>185</v>
       </c>
@@ -4567,7 +4579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:17">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B60" s="4" t="s">
         <v>188</v>
       </c>
@@ -4615,7 +4627,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:17">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B61" s="7" t="s">
         <v>188</v>
       </c>
@@ -4647,7 +4659,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="1:17">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B62" s="4" t="s">
         <v>190</v>
       </c>
@@ -4697,7 +4709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:17">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B63" s="4" t="s">
         <v>194</v>
       </c>
@@ -4747,7 +4759,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="1:17">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B64" s="4" t="s">
         <v>194</v>
       </c>
@@ -4797,7 +4809,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="1:17">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B65" s="4" t="s">
         <v>202</v>
       </c>
@@ -4847,7 +4859,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="1:17">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B66" s="7" t="s">
         <v>202</v>
       </c>
@@ -4881,7 +4893,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="1:17">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B67" s="4" t="s">
         <v>203</v>
       </c>
@@ -4931,7 +4943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:17">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B68" s="4" t="s">
         <v>203</v>
       </c>
@@ -4981,7 +4993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:17">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B69" s="4" t="s">
         <v>210</v>
       </c>
@@ -5031,7 +5043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:17">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B70" s="4" t="s">
         <v>212</v>
       </c>
@@ -5081,7 +5093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:17">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B71" s="4" t="s">
         <v>212</v>
       </c>
@@ -5131,7 +5143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:17">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B72" s="4" t="s">
         <v>218</v>
       </c>
@@ -5181,7 +5193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:17">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B73" s="4" t="s">
         <v>220</v>
       </c>
@@ -5231,7 +5243,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="1:17">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B74" s="4" t="s">
         <v>225</v>
       </c>
@@ -5281,7 +5293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:17">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B75" s="4" t="s">
         <v>225</v>
       </c>
@@ -5331,7 +5343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:17">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B76" s="4" t="s">
         <v>225</v>
       </c>
@@ -5381,7 +5393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:17">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B77" s="4" t="s">
         <v>232</v>
       </c>
@@ -5431,7 +5443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:17">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B78" s="4" t="s">
         <v>232</v>
       </c>
@@ -5481,7 +5493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:17">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>237</v>
       </c>
@@ -5534,7 +5546,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="80" spans="1:17">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>237</v>
       </c>
@@ -5587,7 +5599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:17">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>237</v>
       </c>
@@ -5640,7 +5652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:17">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B82" s="4" t="s">
         <v>246</v>
       </c>
@@ -5690,7 +5702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:17">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B83" s="4" t="s">
         <v>246</v>
       </c>
@@ -5740,7 +5752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:17">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B84" s="4" t="s">
         <v>249</v>
       </c>
@@ -5790,7 +5802,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="1:17">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B85" s="4" t="s">
         <v>254</v>
       </c>
@@ -5840,7 +5852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:17">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B86" s="4" t="s">
         <v>254</v>
       </c>
@@ -5890,7 +5902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:17">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B87" s="4" t="s">
         <v>258</v>
       </c>
@@ -5940,7 +5952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:17">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B88" s="4" t="s">
         <v>258</v>
       </c>
@@ -5990,7 +6002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:17">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B89" s="4" t="s">
         <v>262</v>
       </c>
@@ -6040,7 +6052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:17">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B90" s="4" t="s">
         <v>264</v>
       </c>
@@ -6090,7 +6102,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="91" spans="1:17">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B91" s="4" t="s">
         <v>267</v>
       </c>
@@ -6140,7 +6152,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="92" spans="1:17">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B92" s="4" t="s">
         <v>269</v>
       </c>
@@ -6190,7 +6202,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="93" spans="1:17">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B93" s="4" t="s">
         <v>271</v>
       </c>
@@ -6240,7 +6252,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="94" spans="1:17">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B94" s="4" t="s">
         <v>275</v>
       </c>
@@ -6290,7 +6302,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="95" spans="1:17">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B95" s="4" t="s">
         <v>278</v>
       </c>
@@ -6340,7 +6352,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="96" spans="1:17">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B96" s="4" t="s">
         <v>281</v>
       </c>
@@ -6390,7 +6402,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="97" spans="1:17">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B97" s="4" t="s">
         <v>283</v>
       </c>
@@ -6440,7 +6452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:17">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B98" s="4" t="s">
         <v>286</v>
       </c>
@@ -6488,7 +6500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:17">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B99" s="4" t="s">
         <v>288</v>
       </c>
@@ -6538,7 +6550,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="100" spans="1:17">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B100" s="4" t="s">
         <v>288</v>
       </c>
@@ -6588,7 +6600,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="101" spans="1:17">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>237</v>
       </c>
@@ -6641,7 +6653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:17">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B102" s="4" t="s">
         <v>296</v>
       </c>
@@ -6691,7 +6703,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="103" spans="1:17">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B103" s="4" t="s">
         <v>299</v>
       </c>
@@ -6741,7 +6753,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="104" spans="1:17">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B104" s="4" t="s">
         <v>299</v>
       </c>
@@ -6791,7 +6803,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="105" spans="1:17">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B105" s="4" t="s">
         <v>304</v>
       </c>
@@ -6841,7 +6853,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="106" spans="1:17">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B106" s="4" t="s">
         <v>304</v>
       </c>
@@ -6891,7 +6903,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="107" spans="1:17">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B107" s="4" t="s">
         <v>307</v>
       </c>
@@ -6941,7 +6953,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="108" spans="1:17">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B108" s="4" t="s">
         <v>307</v>
       </c>
@@ -6991,7 +7003,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="109" spans="1:17">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B109" s="4" t="s">
         <v>311</v>
       </c>
@@ -7041,7 +7053,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="110" spans="1:17">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>237</v>
       </c>
@@ -7094,7 +7106,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="111" spans="1:17">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>237</v>
       </c>
@@ -7147,7 +7159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:17">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B112" s="4" t="s">
         <v>318</v>
       </c>
@@ -7197,7 +7209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:17">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>237</v>
       </c>
@@ -7250,7 +7262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:17">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B114" s="4" t="s">
         <v>323</v>
       </c>
@@ -7300,7 +7312,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="115" spans="1:17">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>237</v>
       </c>
@@ -7353,7 +7365,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="116" spans="1:17">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B116" s="4" t="s">
         <v>326</v>
       </c>
@@ -7403,7 +7415,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="117" spans="1:17">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B117" s="4" t="s">
         <v>328</v>
       </c>
@@ -7453,7 +7465,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="118" spans="1:17">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B118" s="4" t="s">
         <v>331</v>
       </c>
@@ -7503,7 +7515,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="119" spans="1:17">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B119" s="4" t="s">
         <v>333</v>
       </c>
@@ -7553,7 +7565,107 @@
         <v>32</v>
       </c>
     </row>
-    <row r="1048576" spans="3:3">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B120" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="C120" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D120" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="E120" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F120" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="G120" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="H120" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I120" s="15">
+        <v>20</v>
+      </c>
+      <c r="J120" s="11">
+        <v>87.39</v>
+      </c>
+      <c r="K120" s="15">
+        <v>28</v>
+      </c>
+      <c r="L120" s="11">
+        <v>49.51</v>
+      </c>
+      <c r="M120" s="21">
+        <v>13.8</v>
+      </c>
+      <c r="N120" s="11">
+        <v>100</v>
+      </c>
+      <c r="O120" s="6">
+        <v>43850</v>
+      </c>
+      <c r="P120" s="25">
+        <v>0.58680555555555558</v>
+      </c>
+      <c r="Q120" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="121" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B121" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="C121" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D121" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="E121" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F121" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="G121" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="H121" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I121" s="15">
+        <v>16</v>
+      </c>
+      <c r="J121" s="11">
+        <v>96.66</v>
+      </c>
+      <c r="K121" s="15">
+        <v>20</v>
+      </c>
+      <c r="L121" s="11">
+        <v>87.39</v>
+      </c>
+      <c r="M121" s="21">
+        <v>11.5</v>
+      </c>
+      <c r="N121" s="11">
+        <v>100</v>
+      </c>
+      <c r="O121" s="6">
+        <v>43850</v>
+      </c>
+      <c r="P121" s="25">
+        <v>0.58680555555555558</v>
+      </c>
+      <c r="Q121" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1048576" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C1048576" s="4" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
0700｜EASY｜Search in a Binary Search Tree
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kzmain/_Repository/👨🏻‍💻LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D4B837-EDD9-6447-8774-DC00B2DD803A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74287FB9-6DB8-3D49-9E96-9DE1F0C72CDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8300" yWindow="2820" windowWidth="21620" windowHeight="11360" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="341">
   <si>
     <t>Date</t>
   </si>
@@ -1197,6 +1197,15 @@
   </si>
   <si>
     <t>string -&gt;  char vector -&gt; Simulate stack</t>
+  </si>
+  <si>
+    <t>Search in a Binary Search Tree</t>
+  </si>
+  <si>
+    <t>0700</t>
+  </si>
+  <si>
+    <t>Tree</t>
   </si>
 </sst>
 </file>
@@ -1634,8 +1643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914384AD-4934-744A-8C44-1EF839F36E18}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C118" sqref="C118"/>
+    <sheetView tabSelected="1" topLeftCell="A113" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7665,6 +7674,56 @@
         <v>28</v>
       </c>
     </row>
+    <row r="122" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B122" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="C122" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D122" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="E122" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F122" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="G122" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="H122" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I122" s="15">
+        <v>44</v>
+      </c>
+      <c r="J122" s="11">
+        <v>96.71</v>
+      </c>
+      <c r="K122" s="15">
+        <v>56</v>
+      </c>
+      <c r="L122" s="11">
+        <v>45.49</v>
+      </c>
+      <c r="M122" s="21">
+        <v>29.3</v>
+      </c>
+      <c r="N122" s="11">
+        <v>9.76</v>
+      </c>
+      <c r="O122" s="6">
+        <v>43850</v>
+      </c>
+      <c r="P122" s="25">
+        <v>0.60138888888888886</v>
+      </c>
+      <c r="Q122" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C1048576" s="4" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
0703｜EASY｜Kth Largest Element in a Stream
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kzmain/_Repository/👨🏻‍💻LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7CA350-9DD9-DA43-AB69-12ECEB70BBD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55490E3-F2DC-6F4C-9E8C-232AB4AEC11F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3500" yWindow="3880" windowWidth="21620" windowHeight="11360" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
+    <workbookView xWindow="13940" yWindow="3360" windowWidth="21620" windowHeight="11360" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="358">
   <si>
     <t>Date</t>
   </si>
@@ -1245,6 +1245,18 @@
   </si>
   <si>
     <t>直接比每个坐下是否相等(他人解法)</t>
+  </si>
+  <si>
+    <t>0703</t>
+  </si>
+  <si>
+    <t>Kth Largest Element in a Stream</t>
+  </si>
+  <si>
+    <t>Heap</t>
+  </si>
+  <si>
+    <t>sort() 方法</t>
   </si>
 </sst>
 </file>
@@ -1682,8 +1694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914384AD-4934-744A-8C44-1EF839F36E18}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H112" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O125" sqref="O125"/>
+    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G132" sqref="G132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8069,6 +8081,90 @@
         <v>0</v>
       </c>
     </row>
+    <row r="129" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B129" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="C129" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D129" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="E129" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F129" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="G129" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="H129" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I129" s="15">
+        <v>200</v>
+      </c>
+      <c r="J129" s="11">
+        <v>12.79</v>
+      </c>
+      <c r="K129" s="15">
+        <v>436</v>
+      </c>
+      <c r="L129" s="11">
+        <v>7.22</v>
+      </c>
+      <c r="M129" s="21">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="N129" s="11">
+        <v>95</v>
+      </c>
+      <c r="O129" s="6">
+        <v>43852</v>
+      </c>
+      <c r="P129" s="25">
+        <v>0.78055555555555556</v>
+      </c>
+      <c r="Q129" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="130" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B130" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="C130" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D130" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="E130" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F130" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="G130" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="H130" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I130" s="16"/>
+      <c r="J130" s="12"/>
+      <c r="K130" s="16"/>
+      <c r="L130" s="12"/>
+      <c r="M130" s="22"/>
+      <c r="N130" s="12"/>
+      <c r="O130" s="28"/>
+      <c r="P130" s="26"/>
+      <c r="Q130" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C1048576" s="4" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
0804｜EASY｜Unique Morse Code Words
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kzmain/_Repository/👨🏻‍💻LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55490E3-F2DC-6F4C-9E8C-232AB4AEC11F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC4E494-5985-764B-B424-F56DE713D05A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13940" yWindow="3360" windowWidth="21620" windowHeight="11360" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="361">
   <si>
     <t>Date</t>
   </si>
@@ -1257,6 +1257,15 @@
   </si>
   <si>
     <t>sort() 方法</t>
+  </si>
+  <si>
+    <t>0804</t>
+  </si>
+  <si>
+    <t>Unique Morse Code Words</t>
+  </si>
+  <si>
+    <t>set</t>
   </si>
 </sst>
 </file>
@@ -1694,8 +1703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914384AD-4934-744A-8C44-1EF839F36E18}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G132" sqref="G132"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C133" sqref="C133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8142,7 +8151,7 @@
         <v>355</v>
       </c>
       <c r="E130" s="8" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="F130" s="8" t="s">
         <v>356</v>
@@ -8165,6 +8174,56 @@
         <v>32</v>
       </c>
     </row>
+    <row r="131" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B131" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="C131" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D131" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="E131" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F131" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G131" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="H131" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I131" s="15">
+        <v>4</v>
+      </c>
+      <c r="J131" s="11">
+        <v>84.08</v>
+      </c>
+      <c r="K131" s="15">
+        <v>4</v>
+      </c>
+      <c r="L131" s="11">
+        <v>84.08</v>
+      </c>
+      <c r="M131" s="21">
+        <v>9</v>
+      </c>
+      <c r="N131" s="11">
+        <v>76.92</v>
+      </c>
+      <c r="O131" s="6">
+        <v>43852</v>
+      </c>
+      <c r="P131" s="25">
+        <v>0.79652777777777783</v>
+      </c>
+      <c r="Q131" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C1048576" s="4" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
0747｜EASY｜Largest Number At Least Twice of Others
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kzmain/_Repository/👨🏻‍💻LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005E2A88-6DAA-CC4A-976D-187B547E8654}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDE228B-DAE7-EA48-96A5-854B3238FB94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13940" yWindow="3360" windowWidth="21620" windowHeight="11360" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
+    <workbookView xWindow="7860" yWindow="5520" windowWidth="21620" windowHeight="11360" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="385">
   <si>
     <t>Date</t>
   </si>
@@ -1302,6 +1302,42 @@
   </si>
   <si>
     <t>iterate</t>
+  </si>
+  <si>
+    <t>0744</t>
+  </si>
+  <si>
+    <t>Find Smallest Letter Greater Than Target</t>
+  </si>
+  <si>
+    <t>普通从头找</t>
+  </si>
+  <si>
+    <t>Min Cost Climbing Stairs</t>
+  </si>
+  <si>
+    <t>0746</t>
+  </si>
+  <si>
+    <t>iteration</t>
+  </si>
+  <si>
+    <t>取前两个中最小一个，虽然是和前一个一样的思想，但是远远比第一个时间少</t>
+  </si>
+  <si>
+    <t>TIMEOUT</t>
+  </si>
+  <si>
+    <t>Largest Number At Least Twice of Others</t>
+  </si>
+  <si>
+    <t>0747</t>
+  </si>
+  <si>
+    <t>在数组中找最大，然后比</t>
+  </si>
+  <si>
+    <t>sort数组，直接取最后两个，看存不存在，存在则一个个去找</t>
   </si>
 </sst>
 </file>
@@ -1739,8 +1775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914384AD-4934-744A-8C44-1EF839F36E18}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D135" sqref="D135"/>
+    <sheetView tabSelected="1" topLeftCell="G131" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K140" sqref="K140:L140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8463,6 +8499,291 @@
         <v>0</v>
       </c>
     </row>
+    <row r="136" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B136" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D136" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="E136" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F136" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G136" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="H136" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I136" s="15">
+        <v>14</v>
+      </c>
+      <c r="J136" s="11">
+        <v>11.17</v>
+      </c>
+      <c r="K136" s="15">
+        <v>14</v>
+      </c>
+      <c r="L136" s="11">
+        <v>11.17</v>
+      </c>
+      <c r="M136" s="21">
+        <v>9.1</v>
+      </c>
+      <c r="N136" s="11">
+        <v>72.73</v>
+      </c>
+      <c r="O136" s="6">
+        <v>43853</v>
+      </c>
+      <c r="P136" s="25">
+        <v>0.18402777777777779</v>
+      </c>
+      <c r="Q136" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A137" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="C137" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D137" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="E137" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F137" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G137" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="H137" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I137" s="16"/>
+      <c r="J137" s="12"/>
+      <c r="K137" s="16"/>
+      <c r="L137" s="12"/>
+      <c r="M137" s="22"/>
+      <c r="N137" s="12"/>
+      <c r="O137" s="28"/>
+      <c r="P137" s="26"/>
+      <c r="Q137" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B138" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C138" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D138" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="E138" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F138" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G138" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="H138" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I138" s="15" t="s">
+        <v>380</v>
+      </c>
+      <c r="J138" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="K138" s="15" t="s">
+        <v>380</v>
+      </c>
+      <c r="L138" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="M138" s="15" t="s">
+        <v>380</v>
+      </c>
+      <c r="N138" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="O138" s="6">
+        <v>43853</v>
+      </c>
+      <c r="P138" s="25">
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="Q138" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B139" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C139" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D139" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="E139" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F139" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G139" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="H139" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I139" s="15">
+        <v>12</v>
+      </c>
+      <c r="J139" s="11">
+        <v>10.76</v>
+      </c>
+      <c r="K139" s="15">
+        <v>12</v>
+      </c>
+      <c r="L139" s="11">
+        <v>10.76</v>
+      </c>
+      <c r="M139" s="21">
+        <v>8.9</v>
+      </c>
+      <c r="N139" s="11">
+        <v>37.21</v>
+      </c>
+      <c r="O139" s="6">
+        <v>43853</v>
+      </c>
+      <c r="P139" s="25">
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="Q139" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B140" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D140" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="E140" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F140" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G140" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="H140" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I140" s="15">
+        <v>16</v>
+      </c>
+      <c r="J140" s="11">
+        <v>7.56</v>
+      </c>
+      <c r="K140" s="15">
+        <v>4</v>
+      </c>
+      <c r="L140" s="11">
+        <v>66.63</v>
+      </c>
+      <c r="M140" s="21">
+        <v>8.5</v>
+      </c>
+      <c r="N140" s="11">
+        <v>50</v>
+      </c>
+      <c r="O140" s="6">
+        <v>43853</v>
+      </c>
+      <c r="P140" s="25">
+        <v>0.58958333333333335</v>
+      </c>
+      <c r="Q140" s="19"/>
+    </row>
+    <row r="141" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B141" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="C141" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D141" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="E141" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F141" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G141" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="H141" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I141" s="15">
+        <v>4</v>
+      </c>
+      <c r="J141" s="11">
+        <v>66.63</v>
+      </c>
+      <c r="K141" s="15">
+        <v>4</v>
+      </c>
+      <c r="L141" s="11">
+        <v>66.63</v>
+      </c>
+      <c r="M141" s="21">
+        <v>8.4</v>
+      </c>
+      <c r="N141" s="11">
+        <v>70</v>
+      </c>
+      <c r="O141" s="6">
+        <v>43853</v>
+      </c>
+      <c r="P141" s="25">
+        <v>0.58958333333333335</v>
+      </c>
+      <c r="Q141" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C1048576" s="4" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
1275｜EASY｜Find Winner on a Tic Tac Toe Game
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kzmain/_Repository/👨🏻‍💻LeetCode/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106181CA-461F-CC45-BE2E-8D170568BFAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B38A04-415E-475B-B125-4D183A78D33E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="2140" windowWidth="33600" windowHeight="19260" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
+    <workbookView xWindow="7185" yWindow="4080" windowWidth="21615" windowHeight="11355" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="396">
   <si>
     <t>Date</t>
   </si>
@@ -1356,6 +1356,26 @@
   </si>
   <si>
     <t>暴力解法</t>
+  </si>
+  <si>
+    <t>1275</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Find Winner on a Tic Tac Toe Game</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>easy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shift 2D Grid</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1260</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1363,28 +1383,28 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="165" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="166" formatCode="[$-F400]hh:mm:ss"/>
+    <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="178" formatCode="[$-F400]hh:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1452,7 +1472,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1468,15 +1488,15 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1793,32 +1813,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914384AD-4934-744A-8C44-1EF839F36E18}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D139" sqref="D139"/>
+    <sheetView tabSelected="1" topLeftCell="H128" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H145" sqref="A145:XFD145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="4.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.125" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.83203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.875" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.125" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="42.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="65.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="65.625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.375" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.625" style="17" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" style="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" style="17" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.1640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.1640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="13.125" style="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.875" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.375" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.125" style="27" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17">
       <c r="A1" s="2" t="s">
         <v>237</v>
       </c>
@@ -1871,7 +1891,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17">
       <c r="B2" s="4" t="s">
         <v>103</v>
       </c>
@@ -1921,7 +1941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17">
       <c r="B3" s="7" t="s">
         <v>103</v>
       </c>
@@ -1953,7 +1973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17">
       <c r="B4" s="4" t="s">
         <v>104</v>
       </c>
@@ -2003,7 +2023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17">
       <c r="B5" s="7" t="s">
         <v>104</v>
       </c>
@@ -2035,7 +2055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17">
       <c r="B6" s="4" t="s">
         <v>105</v>
       </c>
@@ -2085,7 +2105,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17">
       <c r="B7" s="4" t="s">
         <v>106</v>
       </c>
@@ -2135,7 +2155,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17">
       <c r="B8" s="4" t="s">
         <v>107</v>
       </c>
@@ -2185,7 +2205,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17">
       <c r="B9" s="4" t="s">
         <v>108</v>
       </c>
@@ -2235,7 +2255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17">
       <c r="B10" s="4" t="s">
         <v>109</v>
       </c>
@@ -2285,7 +2305,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17">
       <c r="B11" s="4" t="s">
         <v>110</v>
       </c>
@@ -2335,7 +2355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17">
       <c r="B12" s="4" t="s">
         <v>111</v>
       </c>
@@ -2385,7 +2405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17">
       <c r="B13" s="4" t="s">
         <v>112</v>
       </c>
@@ -2435,7 +2455,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17">
       <c r="B14" s="4" t="s">
         <v>113</v>
       </c>
@@ -2485,7 +2505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17">
       <c r="B15" s="4" t="s">
         <v>114</v>
       </c>
@@ -2535,7 +2555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17">
       <c r="B16" s="4" t="s">
         <v>115</v>
       </c>
@@ -2585,7 +2605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:17">
       <c r="B17" s="4" t="s">
         <v>115</v>
       </c>
@@ -2635,7 +2655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:17">
       <c r="B18" s="4" t="s">
         <v>116</v>
       </c>
@@ -2685,7 +2705,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:17">
       <c r="B19" s="4" t="s">
         <v>117</v>
       </c>
@@ -2735,7 +2755,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:17">
       <c r="B20" s="4" t="s">
         <v>118</v>
       </c>
@@ -2785,7 +2805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:17">
       <c r="B21" s="4" t="s">
         <v>119</v>
       </c>
@@ -2835,7 +2855,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:17">
       <c r="B22" s="4" t="s">
         <v>120</v>
       </c>
@@ -2885,7 +2905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:17">
       <c r="B23" s="4" t="s">
         <v>120</v>
       </c>
@@ -2935,7 +2955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:17">
       <c r="B24" s="4" t="s">
         <v>71</v>
       </c>
@@ -2985,7 +3005,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:17">
       <c r="B25" s="4" t="s">
         <v>121</v>
       </c>
@@ -3035,7 +3055,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:17">
       <c r="B26" s="4" t="s">
         <v>122</v>
       </c>
@@ -3085,7 +3105,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:17">
       <c r="B27" s="4" t="s">
         <v>122</v>
       </c>
@@ -3135,7 +3155,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:17">
       <c r="B28" s="4" t="s">
         <v>123</v>
       </c>
@@ -3185,7 +3205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:17">
       <c r="B29" s="4" t="s">
         <v>123</v>
       </c>
@@ -3235,7 +3255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:17">
       <c r="B30" s="4" t="s">
         <v>124</v>
       </c>
@@ -3285,7 +3305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:17">
       <c r="B31" s="4" t="s">
         <v>125</v>
       </c>
@@ -3335,7 +3355,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:17">
       <c r="B32" s="4" t="s">
         <v>126</v>
       </c>
@@ -3385,7 +3405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:17">
       <c r="B33" s="4" t="s">
         <v>127</v>
       </c>
@@ -3435,7 +3455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:17">
       <c r="B34" s="4" t="s">
         <v>128</v>
       </c>
@@ -3485,7 +3505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:17">
       <c r="B35" s="4" t="s">
         <v>128</v>
       </c>
@@ -3535,7 +3555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:17">
       <c r="B36" s="4" t="s">
         <v>129</v>
       </c>
@@ -3585,7 +3605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:17">
       <c r="B37" s="4" t="s">
         <v>129</v>
       </c>
@@ -3635,7 +3655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:17">
       <c r="B38" s="4" t="s">
         <v>130</v>
       </c>
@@ -3685,7 +3705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:17">
       <c r="B39" s="4" t="s">
         <v>133</v>
       </c>
@@ -3735,7 +3755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:17">
       <c r="B40" s="4" t="s">
         <v>137</v>
       </c>
@@ -3785,7 +3805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:17">
       <c r="B41" s="4" t="s">
         <v>137</v>
       </c>
@@ -3835,7 +3855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:17">
       <c r="B42" s="4" t="s">
         <v>156</v>
       </c>
@@ -3885,7 +3905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:17">
       <c r="B43" s="4" t="s">
         <v>156</v>
       </c>
@@ -3935,7 +3955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:17">
       <c r="B44" s="4" t="s">
         <v>157</v>
       </c>
@@ -3985,7 +4005,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:17">
       <c r="B45" s="4" t="s">
         <v>158</v>
       </c>
@@ -4035,7 +4055,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:17">
       <c r="B46" s="4" t="s">
         <v>159</v>
       </c>
@@ -4085,7 +4105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:17">
       <c r="B47" s="4" t="s">
         <v>159</v>
       </c>
@@ -4135,7 +4155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:17">
       <c r="B48" s="4" t="s">
         <v>160</v>
       </c>
@@ -4185,7 +4205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17">
       <c r="B49" s="4" t="s">
         <v>161</v>
       </c>
@@ -4235,7 +4255,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17">
       <c r="B50" s="4" t="s">
         <v>164</v>
       </c>
@@ -4285,7 +4305,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17">
       <c r="B51" s="4" t="s">
         <v>167</v>
       </c>
@@ -4335,7 +4355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17">
       <c r="B52" s="4" t="s">
         <v>167</v>
       </c>
@@ -4385,7 +4405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17">
       <c r="B53" s="4" t="s">
         <v>167</v>
       </c>
@@ -4435,7 +4455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17">
       <c r="B54" s="4" t="s">
         <v>173</v>
       </c>
@@ -4485,7 +4505,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17">
       <c r="A55" s="1" t="s">
         <v>237</v>
       </c>
@@ -4538,7 +4558,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17">
       <c r="B56" s="4" t="s">
         <v>177</v>
       </c>
@@ -4588,7 +4608,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17">
       <c r="B57" s="4" t="s">
         <v>177</v>
       </c>
@@ -4638,7 +4658,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17">
       <c r="B58" s="4" t="s">
         <v>183</v>
       </c>
@@ -4688,7 +4708,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17">
       <c r="B59" s="4" t="s">
         <v>185</v>
       </c>
@@ -4738,7 +4758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17">
       <c r="B60" s="4" t="s">
         <v>188</v>
       </c>
@@ -4786,7 +4806,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17">
       <c r="B61" s="7" t="s">
         <v>188</v>
       </c>
@@ -4818,7 +4838,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:17">
       <c r="B62" s="4" t="s">
         <v>190</v>
       </c>
@@ -4868,7 +4888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17">
       <c r="B63" s="4" t="s">
         <v>194</v>
       </c>
@@ -4918,7 +4938,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:17">
       <c r="B64" s="4" t="s">
         <v>194</v>
       </c>
@@ -4968,7 +4988,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17">
       <c r="B65" s="4" t="s">
         <v>202</v>
       </c>
@@ -5018,7 +5038,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:17">
       <c r="B66" s="7" t="s">
         <v>202</v>
       </c>
@@ -5052,7 +5072,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:17">
       <c r="B67" s="4" t="s">
         <v>203</v>
       </c>
@@ -5102,7 +5122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17">
       <c r="B68" s="4" t="s">
         <v>203</v>
       </c>
@@ -5152,7 +5172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:17">
       <c r="B69" s="4" t="s">
         <v>210</v>
       </c>
@@ -5202,7 +5222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:17">
       <c r="B70" s="4" t="s">
         <v>212</v>
       </c>
@@ -5252,7 +5272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:17">
       <c r="B71" s="4" t="s">
         <v>212</v>
       </c>
@@ -5302,7 +5322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:17">
       <c r="B72" s="4" t="s">
         <v>218</v>
       </c>
@@ -5352,7 +5372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:17">
       <c r="B73" s="4" t="s">
         <v>220</v>
       </c>
@@ -5402,7 +5422,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:17">
       <c r="B74" s="4" t="s">
         <v>225</v>
       </c>
@@ -5452,7 +5472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:17">
       <c r="B75" s="4" t="s">
         <v>225</v>
       </c>
@@ -5502,7 +5522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:17">
       <c r="B76" s="4" t="s">
         <v>225</v>
       </c>
@@ -5552,7 +5572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:17">
       <c r="B77" s="4" t="s">
         <v>232</v>
       </c>
@@ -5602,7 +5622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:17">
       <c r="B78" s="4" t="s">
         <v>232</v>
       </c>
@@ -5652,7 +5672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:17">
       <c r="A79" s="1" t="s">
         <v>237</v>
       </c>
@@ -5705,7 +5725,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:17">
       <c r="A80" s="1" t="s">
         <v>237</v>
       </c>
@@ -5758,7 +5778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:17">
       <c r="A81" s="1" t="s">
         <v>237</v>
       </c>
@@ -5811,7 +5831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:17">
       <c r="B82" s="4" t="s">
         <v>246</v>
       </c>
@@ -5861,7 +5881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:17">
       <c r="B83" s="4" t="s">
         <v>246</v>
       </c>
@@ -5911,7 +5931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:17">
       <c r="B84" s="4" t="s">
         <v>249</v>
       </c>
@@ -5961,7 +5981,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:17">
       <c r="B85" s="4" t="s">
         <v>254</v>
       </c>
@@ -6011,7 +6031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:17">
       <c r="B86" s="4" t="s">
         <v>254</v>
       </c>
@@ -6061,7 +6081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:17">
       <c r="B87" s="4" t="s">
         <v>258</v>
       </c>
@@ -6111,7 +6131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:17">
       <c r="B88" s="4" t="s">
         <v>258</v>
       </c>
@@ -6161,7 +6181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:17">
       <c r="B89" s="4" t="s">
         <v>262</v>
       </c>
@@ -6211,7 +6231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:17">
       <c r="B90" s="4" t="s">
         <v>264</v>
       </c>
@@ -6261,7 +6281,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:17">
       <c r="B91" s="4" t="s">
         <v>267</v>
       </c>
@@ -6311,7 +6331,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:17">
       <c r="B92" s="4" t="s">
         <v>269</v>
       </c>
@@ -6361,7 +6381,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:17">
       <c r="B93" s="4" t="s">
         <v>271</v>
       </c>
@@ -6411,7 +6431,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:17">
       <c r="B94" s="4" t="s">
         <v>275</v>
       </c>
@@ -6461,7 +6481,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:17">
       <c r="B95" s="4" t="s">
         <v>278</v>
       </c>
@@ -6511,7 +6531,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:17">
       <c r="B96" s="4" t="s">
         <v>281</v>
       </c>
@@ -6561,7 +6581,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:17">
       <c r="B97" s="4" t="s">
         <v>283</v>
       </c>
@@ -6611,7 +6631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:17">
       <c r="B98" s="4" t="s">
         <v>286</v>
       </c>
@@ -6659,7 +6679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:17">
       <c r="B99" s="4" t="s">
         <v>288</v>
       </c>
@@ -6709,7 +6729,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:17">
       <c r="B100" s="4" t="s">
         <v>288</v>
       </c>
@@ -6759,7 +6779,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:17">
       <c r="A101" s="1" t="s">
         <v>237</v>
       </c>
@@ -6812,7 +6832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:17">
       <c r="B102" s="4" t="s">
         <v>296</v>
       </c>
@@ -6862,7 +6882,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:17">
       <c r="B103" s="4" t="s">
         <v>299</v>
       </c>
@@ -6912,7 +6932,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:17">
       <c r="B104" s="4" t="s">
         <v>299</v>
       </c>
@@ -6962,7 +6982,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:17">
       <c r="B105" s="4" t="s">
         <v>304</v>
       </c>
@@ -7012,7 +7032,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:17">
       <c r="B106" s="4" t="s">
         <v>304</v>
       </c>
@@ -7062,7 +7082,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:17">
       <c r="B107" s="4" t="s">
         <v>307</v>
       </c>
@@ -7112,7 +7132,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:17">
       <c r="B108" s="4" t="s">
         <v>307</v>
       </c>
@@ -7162,7 +7182,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:17">
       <c r="B109" s="4" t="s">
         <v>311</v>
       </c>
@@ -7212,7 +7232,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:17">
       <c r="A110" s="1" t="s">
         <v>237</v>
       </c>
@@ -7265,7 +7285,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:17">
       <c r="A111" s="1" t="s">
         <v>237</v>
       </c>
@@ -7318,7 +7338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:17">
       <c r="B112" s="4" t="s">
         <v>318</v>
       </c>
@@ -7368,7 +7388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:17">
       <c r="A113" s="1" t="s">
         <v>237</v>
       </c>
@@ -7421,7 +7441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:17">
       <c r="B114" s="4" t="s">
         <v>323</v>
       </c>
@@ -7471,7 +7491,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:17">
       <c r="A115" s="1" t="s">
         <v>237</v>
       </c>
@@ -7524,7 +7544,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:17">
       <c r="B116" s="4" t="s">
         <v>326</v>
       </c>
@@ -7574,7 +7594,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:17">
       <c r="B117" s="4" t="s">
         <v>328</v>
       </c>
@@ -7624,7 +7644,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:17">
       <c r="B118" s="4" t="s">
         <v>331</v>
       </c>
@@ -7674,7 +7694,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:17">
       <c r="B119" s="4" t="s">
         <v>333</v>
       </c>
@@ -7724,7 +7744,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:17">
       <c r="B120" s="4" t="s">
         <v>334</v>
       </c>
@@ -7774,7 +7794,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:17">
       <c r="B121" s="4" t="s">
         <v>334</v>
       </c>
@@ -7824,7 +7844,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:17">
       <c r="B122" s="4" t="s">
         <v>339</v>
       </c>
@@ -7874,7 +7894,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:17">
       <c r="B123" s="4" t="s">
         <v>341</v>
       </c>
@@ -7924,7 +7944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:17">
       <c r="B124" s="4" t="s">
         <v>344</v>
       </c>
@@ -7974,7 +7994,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:17">
       <c r="B125" s="4" t="s">
         <v>347</v>
       </c>
@@ -8024,7 +8044,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:17">
       <c r="B126" s="4" t="s">
         <v>350</v>
       </c>
@@ -8074,7 +8094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:17">
       <c r="A127" s="1" t="s">
         <v>237</v>
       </c>
@@ -8127,7 +8147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:17">
       <c r="A128" s="1" t="s">
         <v>237</v>
       </c>
@@ -8180,7 +8200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:17">
       <c r="B129" s="4" t="s">
         <v>354</v>
       </c>
@@ -8230,7 +8250,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:17">
       <c r="B130" s="7" t="s">
         <v>354</v>
       </c>
@@ -8264,7 +8284,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:17">
       <c r="B131" s="4" t="s">
         <v>358</v>
       </c>
@@ -8314,7 +8334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:17">
       <c r="B132" s="4" t="s">
         <v>362</v>
       </c>
@@ -8364,7 +8384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:17">
       <c r="A133" s="1" t="s">
         <v>237</v>
       </c>
@@ -8417,7 +8437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:17">
       <c r="B134" s="4" t="s">
         <v>366</v>
       </c>
@@ -8467,7 +8487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:17">
       <c r="B135" s="4" t="s">
         <v>370</v>
       </c>
@@ -8517,7 +8537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:17">
       <c r="B136" s="4" t="s">
         <v>373</v>
       </c>
@@ -8567,7 +8587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:17">
       <c r="A137" s="1" t="s">
         <v>237</v>
       </c>
@@ -8604,7 +8624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:17">
       <c r="B138" s="4" t="s">
         <v>377</v>
       </c>
@@ -8654,7 +8674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:17">
       <c r="B139" s="4" t="s">
         <v>377</v>
       </c>
@@ -8704,7 +8724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:17">
       <c r="B140" s="4" t="s">
         <v>382</v>
       </c>
@@ -8752,7 +8772,7 @@
       </c>
       <c r="Q140" s="19"/>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:17">
       <c r="B141" s="4" t="s">
         <v>382</v>
       </c>
@@ -8802,7 +8822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:17">
       <c r="B142" s="4" t="s">
         <v>386</v>
       </c>
@@ -8850,7 +8870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:17">
       <c r="B143" s="4" t="s">
         <v>389</v>
       </c>
@@ -8900,7 +8920,107 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1048576" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:17">
+      <c r="B144" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="C144" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D144" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="E144" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F144" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G144" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="H144" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I144" s="15">
+        <v>12</v>
+      </c>
+      <c r="J144" s="11">
+        <v>59.62</v>
+      </c>
+      <c r="K144" s="15">
+        <v>12</v>
+      </c>
+      <c r="L144" s="11">
+        <v>59.62</v>
+      </c>
+      <c r="M144" s="21">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="N144" s="11">
+        <v>100</v>
+      </c>
+      <c r="O144" s="6">
+        <v>43854</v>
+      </c>
+      <c r="P144" s="25">
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="Q144" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="145" spans="2:17">
+      <c r="B145" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="C145" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D145" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="E145" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F145" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G145" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="H145" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I145" s="15">
+        <v>68</v>
+      </c>
+      <c r="J145" s="11">
+        <v>76.19</v>
+      </c>
+      <c r="K145" s="15">
+        <v>72</v>
+      </c>
+      <c r="L145" s="11">
+        <v>52.27</v>
+      </c>
+      <c r="M145" s="21">
+        <v>13.3</v>
+      </c>
+      <c r="N145" s="11">
+        <v>100</v>
+      </c>
+      <c r="O145" s="6">
+        <v>43854</v>
+      </c>
+      <c r="P145" s="25">
+        <v>0.60833333333333328</v>
+      </c>
+      <c r="Q145" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1048576" spans="3:3">
       <c r="C1048576" s="4" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
1252｜EASY｜Cells with Odd Values in a Matrix
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B38A04-415E-475B-B125-4D183A78D33E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227E9A14-622C-4101-8E4D-80DA59037701}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7185" yWindow="4080" windowWidth="21615" windowHeight="11355" xr2:uid="{9D32CD73-66AA-DF45-930B-57BFCDBED0FA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="398">
   <si>
     <t>Date</t>
   </si>
@@ -1375,6 +1375,14 @@
   </si>
   <si>
     <t>1260</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cells with Odd Values in a Matrix</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1252</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1813,8 +1821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914384AD-4934-744A-8C44-1EF839F36E18}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H128" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H145" sqref="A145:XFD145"/>
+    <sheetView tabSelected="1" topLeftCell="H137" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J144" sqref="J144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -9020,6 +9028,56 @@
         <v>0</v>
       </c>
     </row>
+    <row r="146" spans="2:17">
+      <c r="B146" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="C146" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D146" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="E146" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F146" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G146" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="H146" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I146" s="15">
+        <v>4</v>
+      </c>
+      <c r="J146" s="11">
+        <v>82.63</v>
+      </c>
+      <c r="K146" s="15">
+        <v>8</v>
+      </c>
+      <c r="L146" s="11">
+        <v>29.48</v>
+      </c>
+      <c r="M146" s="21">
+        <v>9.5</v>
+      </c>
+      <c r="N146" s="11">
+        <v>100</v>
+      </c>
+      <c r="O146" s="6">
+        <v>43854</v>
+      </c>
+      <c r="P146" s="25">
+        <v>0.64861111111111114</v>
+      </c>
+      <c r="Q146" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
     <row r="1048576" spans="3:3">
       <c r="C1048576" s="4" t="s">
         <v>94</v>

</xml_diff>